<commit_message>
Modif midi Mercredi 03/07
Création evo moyenne stats bomb + creation moyenne avec evolution en % metriques
</commit_message>
<xml_diff>
--- a/Tableau métriques/Evolutions métriques/evo_passes.xlsx
+++ b/Tableau métriques/Evolutions métriques/evo_passes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabie\Documents\Programmation\Github\Stage CF63\Tableau métriques\Evolutions métriques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3A49D1-99AD-4F11-9A10-F524E2A63191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11CD026-832D-4245-9A2B-CF3544ADAE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,15 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
-  <si>
-    <t>passes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>2021_2022</t>
   </si>
@@ -65,6 +61,9 @@
     <t>pass_opportunities_to_dropping_off_runs_threat_per_match</t>
   </si>
   <si>
+    <t>count_completed_pass_to_pulling_half_space_runs_leading_to_goal_per_match</t>
+  </si>
+  <si>
     <t>count_completed_pass_to_underlap_runs_leading_to_shot_per_match</t>
   </si>
   <si>
@@ -83,9 +82,6 @@
     <t>count_completed_pass_to_dangerous_underlap_runs_per_match</t>
   </si>
   <si>
-    <t>count_opportunities_to_pass_to_dropping_off_runs_in_sample</t>
-  </si>
-  <si>
     <t>count_opportunities_to_pass_to_dropping_off_runs_per_match</t>
   </si>
   <si>
@@ -104,9 +100,6 @@
     <t>underlap_runs_to_which_pass_completed_threat_per_match</t>
   </si>
   <si>
-    <t>count_opportunities_to_pass_to_underlap_runs_in_sample</t>
-  </si>
-  <si>
     <t>count_opportunities_to_pass_to_underlap_runs_per_match</t>
   </si>
   <si>
@@ -128,334 +121,307 @@
     <t>underlap_runs_to_which_pass_attempted_threat_per_match</t>
   </si>
   <si>
+    <t>count_completed_pass_to_underlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_cross_receiver_runs_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>cross_receiver_runs_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_dangerous_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_runs_in_behind_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_runs_in_behind_leading_to_goal_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_underlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_cross_receiver_runs_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_opportunities_to_dangerous_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_cross_receiver_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>cross_receiver_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_coming_short_runs_by_teammate_per_match</t>
+  </si>
+  <si>
     <t>pass_completion_ratio_to_dropping_off_runs</t>
   </si>
   <si>
-    <t>count_completed_pass_to_underlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_cross_receiver_runs_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>cross_receiver_runs_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_dangerous_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_runs_in_behind_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_runs_in_behind_leading_to_goal_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_underlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_cross_receiver_runs_in_sample</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_cross_receiver_runs_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dangerous_cross_receiver_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_coming_short_runs_per_match</t>
+    <t>count_pass_opportunities_to_dangerous_overlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_overlap_runs_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_coming_short_runs_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>support_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_support_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_runs_in_behind_per_match</t>
   </si>
   <si>
     <t>pass_completion_ratio_to_underlap_runs</t>
   </si>
   <si>
-    <t>count_pass_attempts_to_coming_short_runs_per_match</t>
-  </si>
-  <si>
-    <t>cross_receiver_runs_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_coming_short_runs_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_overlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_coming_short_runs_in_sample</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_coming_short_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_overlap_runs_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_coming_short_runs_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>support_runs_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dangerous_support_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_runs_in_behind_per_match</t>
-  </si>
-  <si>
     <t>count_completed_pass_to_support_runs_leading_to_shot_per_match</t>
   </si>
   <si>
     <t>count_pass_attempts_to_dangerous_overlap_runs_per_match</t>
   </si>
   <si>
+    <t>count_completed_pass_to_runs_ahead_of_the_ball_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>overlap_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_overlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>pulling_wide_runs_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_overlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>overlap_runs_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_support_runs_per_match</t>
+  </si>
+  <si>
+    <t>runs_in_behind_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>pulling_wide_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_opportunities_to_dangerous_dropping_off_runs_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_pulling_wide_runs_threat_per_match</t>
+  </si>
+  <si>
+    <t>coming_short_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_overlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_opportunities_to_dangerous_support_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_overlap_runs_leading_to_goal_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_overlap_runs_threat_per_match</t>
+  </si>
+  <si>
+    <t>coming_short_runs_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_support_runs_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_support_runs_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_support_runs_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_runs_ahead_of_the_ball_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_runs_ahead_of_the_ball_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_support_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_runs_in_behind_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_runs_in_behind_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_overlap_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>support_runs_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_runs_in_behind_per_match</t>
+  </si>
+  <si>
+    <t>count_pulling_wide_runs_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>count_overlap_runs_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_coming_short_runs_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_runs_in_behind_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_pulling_wide_runs_per_match</t>
+  </si>
+  <si>
     <t>pass_completion_ratio_to_cross_receiver_runs</t>
   </si>
   <si>
-    <t>count_completed_pass_to_runs_ahead_of_the_ball_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>overlap_runs_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_overlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>pulling_wide_runs_to_which_pass_attempted_threat_per_match</t>
+    <t>count_completed_pass_to_runs_ahead_of_the_ball_leading_to_goal_per_match</t>
+  </si>
+  <si>
+    <t>runs_ahead_of_the_ball_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_pulling_wide_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_opportunities_to_pass_to_runs_ahead_of_the_ball_per_match</t>
+  </si>
+  <si>
+    <t>runs_ahead_of_the_ball_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_runs_in_behind_threat_per_match</t>
   </si>
   <si>
     <t>pass_completion_ratio_to_runs_in_behind</t>
   </si>
   <si>
-    <t>count_completed_pass_to_dangerous_overlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>overlap_runs_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_support_runs_per_match</t>
-  </si>
-  <si>
-    <t>runs_in_behind_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>pulling_wide_runs_to_which_pass_completed_threat_per_match</t>
+    <t>count_runs_ahead_of_the_ball_by_teammate_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_pulling_wide_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_support_runs_leading_to_goal_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dangerous_runs_ahead_of_the_ball_per_match</t>
   </si>
   <si>
     <t>pass_completion_ratio_to_overlap_runs</t>
   </si>
   <si>
+    <t>count_completed_pass_to_pulling_wide_runs_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>runs_in_behind_to_which_pass_attempted_threat_per_match</t>
+  </si>
+  <si>
     <t>pass_completion_ratio_to_coming_short_runs</t>
   </si>
   <si>
-    <t>count_pass_opportunities_to_dangerous_dropping_off_runs_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_pulling_wide_runs_threat_per_match</t>
-  </si>
-  <si>
-    <t>coming_short_runs_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_overlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_support_runs_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_overlap_runs_threat_per_match</t>
-  </si>
-  <si>
-    <t>coming_short_runs_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_support_runs_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_support_runs_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_support_runs_by_teammate_per_match</t>
+    <t>count_pass_opportunities_to_dangerous_runs_in_behind_per_match</t>
+  </si>
+  <si>
+    <t>pass_opportunities_to_runs_ahead_of_the_ball_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_dangerous_pulling_half_space_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_dangerous_runs_ahead_of_the_ball_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_dangerous_support_runs_per_match</t>
   </si>
   <si>
     <t>pass_completion_ratio_to_support_runs</t>
   </si>
   <si>
-    <t>count_pass_attempts_to_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_support_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_support_runs_in_sample</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dangerous_runs_in_behind_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_runs_in_behind_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_overlap_runs_in_sample</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_overlap_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dangerous_coming_short_runs_per_match</t>
-  </si>
-  <si>
-    <t>support_runs_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_runs_in_behind_in_sample</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_runs_in_behind_per_match</t>
-  </si>
-  <si>
-    <t>count_pulling_wide_runs_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_overlap_runs_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_coming_short_runs_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_runs_in_behind_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_pulling_wide_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_runs_ahead_of_the_ball_leading_to_goal_per_match</t>
-  </si>
-  <si>
-    <t>runs_ahead_of_the_ball_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_pulling_wide_runs_in_sample</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_pulling_wide_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_runs_ahead_of_the_ball_in_sample</t>
-  </si>
-  <si>
-    <t>count_opportunities_to_pass_to_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>runs_ahead_of_the_ball_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_runs_in_behind_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_runs_ahead_of_the_ball_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_pulling_wide_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_support_runs_leading_to_goal_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dangerous_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_pulling_wide_runs_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>runs_in_behind_to_which_pass_attempted_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_runs_in_behind_per_match</t>
-  </si>
-  <si>
-    <t>pass_opportunities_to_runs_ahead_of_the_ball_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_dangerous_pulling_half_space_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_dangerous_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_dangerous_support_runs_per_match</t>
+    <t>count_pass_attempts_to_dangerous_runs_in_behind_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_opportunities_to_dangerous_pulling_half_space_runs_per_match</t>
+  </si>
+  <si>
+    <t>pulling_half_space_runs_to_which_pass_completed_threat_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_opportunities_to_dangerous_runs_ahead_of_the_ball_per_match</t>
+  </si>
+  <si>
+    <t>pass_completion_ratio_to_pulling_half_space_runs</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_pulling_half_space_runs_leading_to_shot_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_dangerous_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_completed_pass_to_dropping_off_runs_leading_to_goal_per_match</t>
   </si>
   <si>
     <t>pass_completion_ratio_to_runs_ahead_of_the_ball</t>
   </si>
   <si>
+    <t>count_pass_opportunities_to_dangerous_coming_short_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_pass_attempts_to_pulling_half_space_runs_per_match</t>
+  </si>
+  <si>
     <t>pass_completion_ratio_to_pulling_wide_runs</t>
   </si>
   <si>
-    <t>count_pass_attempts_to_dangerous_runs_in_behind_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_pulling_half_space_runs_per_match</t>
-  </si>
-  <si>
-    <t>pulling_half_space_runs_to_which_pass_completed_threat_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_runs_ahead_of_the_ball_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_pulling_half_space_runs_leading_to_shot_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_dangerous_coming_short_runs_per_match</t>
-  </si>
-  <si>
     <t>pass_opportunities_to_pulling_half_space_runs_threat_per_match</t>
   </si>
   <si>
     <t>pulling_half_space_runs_to_which_pass_attempted_threat_per_match</t>
   </si>
   <si>
-    <t>count_opportunities_to_pass_to_pulling_half_space_runs_in_sample</t>
+    <t>count_completed_pass_to_pulling_half_space_runs_per_match</t>
+  </si>
+  <si>
+    <t>count_pulling_half_space_runs_by_teammate_per_match</t>
   </si>
   <si>
     <t>count_opportunities_to_pass_to_pulling_half_space_runs_per_match</t>
-  </si>
-  <si>
-    <t>pass_completion_ratio_to_pulling_half_space_runs</t>
-  </si>
-  <si>
-    <t>count_pulling_half_space_runs_by_teammate_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_pulling_half_space_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_attempts_to_pulling_half_space_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_pass_opportunities_to_dangerous_coming_short_runs_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_dropping_off_runs_leading_to_goal_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_overlap_runs_leading_to_goal_per_match</t>
-  </si>
-  <si>
-    <t>count_completed_pass_to_pulling_half_space_runs_leading_to_goal_per_match</t>
   </si>
 </sst>
 </file>
@@ -818,37 +784,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.44140625" customWidth="1"/>
+    <col min="1" max="1" width="88.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>8.2383220541115288E-3</v>
@@ -860,12 +826,12 @@
         <v>2.5436468857521492E-2</v>
       </c>
       <c r="E2">
-        <v>208.75788407454669</v>
+        <v>208.76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.257738881577891E-2</v>
@@ -877,12 +843,12 @@
         <v>3.7715194952037047E-2</v>
       </c>
       <c r="E3">
-        <v>199.8650634440244</v>
+        <v>199.87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>5.6484013062960432E-3</v>
@@ -891,18 +857,18 @@
         <v>7.2712418300653597E-3</v>
       </c>
       <c r="D4">
-        <v>1.2094989726568681E-2</v>
+        <v>1.209498972656867E-2</v>
       </c>
       <c r="E4">
-        <v>114.1312040468315</v>
+        <v>114.13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>7.098404614658485E-2</v>
+        <v>7.0984046146584837E-2</v>
       </c>
       <c r="C5">
         <v>0.1083790536344716</v>
@@ -911,29 +877,29 @@
         <v>0.12555181699918541</v>
       </c>
       <c r="E5">
-        <v>76.873288879470124</v>
+        <v>76.87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>1.4529980253664469E-2</v>
+        <v>1.4529980253664461E-2</v>
       </c>
       <c r="C6">
-        <v>5.8751608751608751E-3</v>
+        <v>5.8751608751608743E-3</v>
       </c>
       <c r="D6">
         <v>2.5250908803540379E-2</v>
       </c>
       <c r="E6">
-        <v>73.78488038324825</v>
+        <v>73.78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1.105775803144224E-2</v>
@@ -945,12 +911,12 @@
         <v>1.867196143511933E-2</v>
       </c>
       <c r="E7">
-        <v>68.858473679985039</v>
+        <v>68.86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5.6484013062960432E-3</v>
@@ -962,12 +928,12 @@
         <v>9.3547494863284349E-3</v>
       </c>
       <c r="E8">
-        <v>65.617649650726406</v>
+        <v>65.62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1.477350410399946E-2</v>
@@ -979,165 +945,165 @@
         <v>2.41544175754702E-2</v>
       </c>
       <c r="E9">
-        <v>63.498229028353272</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>5.4661855526793608E-3</v>
+        <v>5.466185552679359E-3</v>
       </c>
       <c r="C10">
-        <v>6.6301854687303586E-3</v>
+        <v>6.6301854687303612E-3</v>
       </c>
       <c r="D10">
-        <v>8.5619886080412419E-3</v>
+        <v>8.5619886080412402E-3</v>
       </c>
       <c r="E10">
-        <v>56.635528112367332</v>
+        <v>56.64</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>0.15695277300540461</v>
+        <v>1.801294740923224E-2</v>
       </c>
       <c r="C11">
-        <v>0.1915016388468401</v>
+        <v>1.6099485658309189E-2</v>
       </c>
       <c r="D11">
-        <v>0.23906320287899241</v>
+        <v>7.8965605281394752E-3</v>
       </c>
       <c r="E11">
-        <v>52.315373791299812</v>
+        <v>-56.16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>1.8655534166370079E-3</v>
+        <v>0.15695277300540461</v>
       </c>
       <c r="C12">
-        <v>2.258665238154402E-3</v>
+        <v>0.1915016388468401</v>
       </c>
       <c r="D12">
-        <v>2.8263364579154049E-3</v>
+        <v>0.23906320287899241</v>
       </c>
       <c r="E12">
-        <v>51.501234577907667</v>
+        <v>52.32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>6.7189767319836973</v>
+        <v>1.8655534166370071E-3</v>
       </c>
       <c r="C13">
-        <v>7.677797419368626</v>
+        <v>2.2586652381544029E-3</v>
       </c>
       <c r="D13">
-        <v>10.07654967720757</v>
+        <v>2.8263364579154049E-3</v>
       </c>
       <c r="E13">
-        <v>49.971492373848292</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>2.9023306771720092</v>
+        <v>6.718976731983699</v>
       </c>
       <c r="C14">
-        <v>3.3457542634709818</v>
+        <v>7.677797419368626</v>
       </c>
       <c r="D14">
-        <v>4.3394356907514799</v>
+        <v>10.07654967720757</v>
       </c>
       <c r="E14">
-        <v>49.515550549869353</v>
+        <v>49.97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>3.0358140413635768</v>
+        <v>2.9023306771720079</v>
       </c>
       <c r="C15">
-        <v>3.486609366795125</v>
+        <v>3.3457542634709809</v>
       </c>
       <c r="D15">
-        <v>4.5249489367910423</v>
+        <v>4.3394356907514799</v>
       </c>
       <c r="E15">
-        <v>49.052243488491158</v>
+        <v>49.52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>0.2855802809556679</v>
+        <v>3.0358140413635768</v>
       </c>
       <c r="C16">
-        <v>0.28163495800492699</v>
+        <v>3.486609366795125</v>
       </c>
       <c r="D16">
-        <v>0.42516717121980269</v>
+        <v>4.5249489367910423</v>
       </c>
       <c r="E16">
-        <v>48.878336346270217</v>
+        <v>49.05</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>6.4590857007072184</v>
+        <v>0.28558028095566801</v>
       </c>
       <c r="C17">
-        <v>7.3345630785181868</v>
+        <v>0.28163495800492699</v>
       </c>
       <c r="D17">
-        <v>9.5887575834944236</v>
+        <v>0.42516717121980269</v>
       </c>
       <c r="E17">
-        <v>48.453790951318886</v>
+        <v>48.88</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6.4590857007072184</v>
       </c>
       <c r="C18">
-        <v>7.3345630785181886</v>
+        <v>7.3345630785181868</v>
       </c>
       <c r="D18">
         <v>9.5887575834944236</v>
       </c>
       <c r="E18">
-        <v>48.453790951318872</v>
+        <v>48.45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1.01019461443223</v>
@@ -1149,15 +1115,15 @@
         <v>1.488756671651408</v>
       </c>
       <c r="E19">
-        <v>47.373253666388727</v>
+        <v>47.37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>2.194559221726405E-3</v>
+        <v>2.1945592217264042E-3</v>
       </c>
       <c r="C20">
         <v>2.6077233841939719E-3</v>
@@ -1166,46 +1132,46 @@
         <v>3.2283999586631171E-3</v>
       </c>
       <c r="E20">
-        <v>47.10926580160433</v>
+        <v>47.11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>3.0919473462043118E-2</v>
       </c>
       <c r="C21">
-        <v>2.263622755882818E-2</v>
+        <v>2.263622755882817E-2</v>
       </c>
       <c r="D21">
         <v>4.5060698350172033E-2</v>
       </c>
       <c r="E21">
-        <v>45.735658808966242</v>
+        <v>45.74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>5.9754436245844908E-2</v>
+        <v>5.9754436245844922E-2</v>
       </c>
       <c r="C22">
         <v>6.7844027424754982E-2</v>
       </c>
       <c r="D22">
-        <v>8.5865259996838972E-2</v>
+        <v>8.5865259996838944E-2</v>
       </c>
       <c r="E22">
-        <v>43.696879079517231</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1.775322914100004E-2</v>
@@ -1217,12 +1183,12 @@
         <v>2.5510098661414449E-2</v>
       </c>
       <c r="E23">
-        <v>43.692724623828447</v>
+        <v>43.69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>3.1217573459833519</v>
@@ -1231,1999 +1197,1829 @@
         <v>3.5582541877046521</v>
       </c>
       <c r="D24">
-        <v>4.4200269601585376</v>
+        <v>4.4200269601585394</v>
       </c>
       <c r="E24">
-        <v>41.587781185030948</v>
+        <v>41.59</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
-        <v>3.1217573459833532</v>
+        <v>0.18652348729748111</v>
       </c>
       <c r="C25">
-        <v>3.558254187704653</v>
+        <v>0.21016108132981201</v>
       </c>
       <c r="D25">
-        <v>4.4200269601585376</v>
+        <v>0.26407505683821481</v>
       </c>
       <c r="E25">
-        <v>41.587781185030927</v>
+        <v>41.58</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <v>0.18652348729748111</v>
+        <v>3.1797474222242021</v>
       </c>
       <c r="C26">
-        <v>0.21016108132981201</v>
+        <v>3.6174979241233109</v>
       </c>
       <c r="D26">
-        <v>0.26407505683821481</v>
+        <v>4.497108849740429</v>
       </c>
       <c r="E26">
-        <v>41.577374873465047</v>
+        <v>41.43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>3.1797474222242021</v>
+        <v>8.7520712617461832E-2</v>
       </c>
       <c r="C27">
-        <v>3.6174979241233109</v>
+        <v>8.3384001387097367E-2</v>
       </c>
       <c r="D27">
-        <v>4.4971088497404281</v>
+        <v>0.12241249346512501</v>
       </c>
       <c r="E27">
-        <v>41.429750624492833</v>
+        <v>39.869999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>8.7520712617461832E-2</v>
+        <v>0.48300370713296409</v>
       </c>
       <c r="C28">
-        <v>8.3384001387097353E-2</v>
+        <v>0.50492379024112766</v>
       </c>
       <c r="D28">
-        <v>0.1224124934651251</v>
+        <v>0.67516549950760474</v>
       </c>
       <c r="E28">
-        <v>39.866883854304611</v>
+        <v>39.78</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>0.48300370713296409</v>
+        <v>0.92134451940179485</v>
       </c>
       <c r="C29">
-        <v>0.50492379024112766</v>
+        <v>1.0295550050271409</v>
       </c>
       <c r="D29">
-        <v>0.67516549950760463</v>
+        <v>1.2848792111950009</v>
       </c>
       <c r="E29">
-        <v>39.784744824275457</v>
+        <v>39.46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>0.92134451940179507</v>
+        <v>2.819750031739196E-2</v>
       </c>
       <c r="C30">
-        <v>1.0295550050271409</v>
+        <v>2.9956724023287491E-2</v>
       </c>
       <c r="D30">
-        <v>1.2848792111950009</v>
+        <v>3.9222934979513922E-2</v>
       </c>
       <c r="E30">
-        <v>39.456976639882683</v>
+        <v>39.1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
-        <v>2.819750031739196E-2</v>
+        <v>0.95922406494387924</v>
       </c>
       <c r="C31">
-        <v>2.9956724023287491E-2</v>
+        <v>0.99694406410350678</v>
       </c>
       <c r="D31">
-        <v>3.9222934979513929E-2</v>
+        <v>1.298893174551069</v>
       </c>
       <c r="E31">
-        <v>39.100751974534361</v>
+        <v>35.409999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>213.65590117602949</v>
+        <v>14.73008751168968</v>
       </c>
       <c r="C32">
-        <v>240.20614300715721</v>
+        <v>16.20174675771425</v>
       </c>
       <c r="D32">
-        <v>293.3987365867892</v>
+        <v>19.73999145907041</v>
       </c>
       <c r="E32">
-        <v>37.323020319977097</v>
+        <v>34.01</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
-        <v>0.95922406494387913</v>
+        <v>5.1130795283310757</v>
       </c>
       <c r="C33">
-        <v>0.99694406410350678</v>
+        <v>5.6668023053007577</v>
       </c>
       <c r="D33">
-        <v>1.298893174551069</v>
+        <v>6.811211717790667</v>
       </c>
       <c r="E33">
-        <v>35.410820268261617</v>
+        <v>33.21</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
-        <v>14.73008751168968</v>
+        <v>0.40181275943501182</v>
       </c>
       <c r="C34">
-        <v>16.20174675771425</v>
+        <v>0.44819359814057969</v>
       </c>
       <c r="D34">
-        <v>19.73999145907041</v>
+        <v>0.53497661274634956</v>
       </c>
       <c r="E34">
-        <v>34.01136580760236</v>
+        <v>33.14</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
-        <v>5.1130795283310757</v>
+        <v>4.9178539362208094</v>
       </c>
       <c r="C35">
-        <v>5.6668023053007568</v>
+        <v>5.4485487439512212</v>
       </c>
       <c r="D35">
-        <v>6.811211717790667</v>
+        <v>6.5275882664040568</v>
       </c>
       <c r="E35">
-        <v>33.211534849994138</v>
+        <v>32.729999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>0.40181275943501182</v>
+        <v>1.056985524876392</v>
       </c>
       <c r="C36">
-        <v>0.44819359814057957</v>
+        <v>1.16475160114479</v>
       </c>
       <c r="D36">
-        <v>0.53497661274634956</v>
+        <v>1.396601713049082</v>
       </c>
       <c r="E36">
-        <v>33.140772706814779</v>
+        <v>32.130000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
-        <v>4.9178539362208094</v>
+        <v>0.17669627615061051</v>
       </c>
       <c r="C37">
-        <v>5.4485487439512221</v>
+        <v>0.18452155313610419</v>
       </c>
       <c r="D37">
-        <v>6.527588266404055</v>
+        <v>0.23345810385284069</v>
       </c>
       <c r="E37">
-        <v>32.732455072064766</v>
+        <v>32.119999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
-        <v>1.056985524876392</v>
+        <v>1.492397079138565</v>
       </c>
       <c r="C38">
-        <v>1.16475160114479</v>
+        <v>1.5530141925730161</v>
       </c>
       <c r="D38">
-        <v>1.396601713049082</v>
+        <v>1.9690634460371299</v>
       </c>
       <c r="E38">
-        <v>32.130637570690112</v>
+        <v>31.94</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
-        <v>0.17669627615061051</v>
+        <v>1.9372122950683319</v>
       </c>
       <c r="C39">
-        <v>0.18452155313610419</v>
+        <v>2.0820113065701298</v>
       </c>
       <c r="D39">
-        <v>0.23345810385284069</v>
+        <v>2.554778513331144</v>
       </c>
       <c r="E39">
-        <v>32.123952433410743</v>
+        <v>31.88</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40">
-        <v>1.492397079138565</v>
+        <v>9.6892967280235069</v>
       </c>
       <c r="C40">
-        <v>1.5530141925730161</v>
+        <v>10.67596248685258</v>
       </c>
       <c r="D40">
-        <v>1.9690634460371299</v>
+        <v>12.70995459021775</v>
       </c>
       <c r="E40">
-        <v>31.939647534937841</v>
+        <v>31.18</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>1.9372122950683319</v>
+        <v>0.69919254158155097</v>
       </c>
       <c r="C41">
-        <v>2.0820113065701298</v>
+        <v>0.77056814292077447</v>
       </c>
       <c r="D41">
-        <v>2.554778513331144</v>
+        <v>0.91615224434961262</v>
       </c>
       <c r="E41">
-        <v>31.879119280575718</v>
+        <v>31.03</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>9.6892967280235105</v>
+        <v>9.2352248067689242</v>
       </c>
       <c r="C42">
-        <v>10.67596248685258</v>
+        <v>10.205566456247571</v>
       </c>
       <c r="D42">
-        <v>12.70995459021775</v>
+        <v>12.08003261358524</v>
       </c>
       <c r="E42">
-        <v>31.17520235971153</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43">
-        <v>9.6892967280235087</v>
+        <v>1.8328397487027519</v>
       </c>
       <c r="C43">
-        <v>10.67596248685258</v>
+        <v>1.959689036871699</v>
       </c>
       <c r="D43">
-        <v>12.709954590217739</v>
+        <v>2.3964465477623369</v>
       </c>
       <c r="E43">
-        <v>31.17520235971152</v>
+        <v>30.75</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44">
-        <v>0.69919254158155097</v>
+        <v>6.1615098254068847</v>
       </c>
       <c r="C44">
-        <v>0.77056814292077447</v>
+        <v>6.6544420621820013</v>
       </c>
       <c r="D44">
-        <v>0.91615224434961262</v>
+        <v>8.0185813850287548</v>
       </c>
       <c r="E44">
-        <v>31.030036773176359</v>
+        <v>30.14</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
-        <v>9.2352248067689242</v>
+        <v>6.8136815237124848</v>
       </c>
       <c r="C45">
-        <v>10.205566456247571</v>
+        <v>7.3039452686975892</v>
       </c>
       <c r="D45">
-        <v>12.08003261358524</v>
+        <v>8.8255743091269405</v>
       </c>
       <c r="E45">
-        <v>30.803882594511691</v>
+        <v>29.53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46">
-        <v>1.8328397487027519</v>
+        <v>0.1446676027484077</v>
       </c>
       <c r="C46">
-        <v>1.959689036871699</v>
+        <v>0.1501832224247085</v>
       </c>
       <c r="D46">
-        <v>2.3964465477623378</v>
+        <v>0.18637674010042429</v>
       </c>
       <c r="E46">
-        <v>30.750467925987301</v>
+        <v>28.83</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47">
-        <v>6.161509825406883</v>
+        <v>16.916112328863878</v>
       </c>
       <c r="C47">
-        <v>6.6544420621820013</v>
+        <v>18.116406844905288</v>
       </c>
       <c r="D47">
-        <v>8.0185813850287531</v>
+        <v>21.643883964936599</v>
       </c>
       <c r="E47">
-        <v>30.13987824809216</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48">
-        <v>83.698797758308359</v>
+        <v>16.33062108541068</v>
       </c>
       <c r="C48">
-        <v>83.947694044132589</v>
+        <v>17.784115810267309</v>
       </c>
       <c r="D48">
-        <v>108.79282878171691</v>
+        <v>20.884734830210839</v>
       </c>
       <c r="E48">
-        <v>29.98135181806434</v>
+        <v>27.89</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>6.8136815237124839</v>
+        <v>1.1112997670544109</v>
       </c>
       <c r="C49">
-        <v>7.303945268697591</v>
+        <v>1.2069481117159131</v>
       </c>
       <c r="D49">
-        <v>8.8255743091269405</v>
+        <v>1.410100181152812</v>
       </c>
       <c r="E49">
-        <v>29.527250113067549</v>
+        <v>26.89</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>0.1446676027484077</v>
+        <v>16.029834853282999</v>
       </c>
       <c r="C50">
-        <v>0.1501832224247085</v>
+        <v>17.083656953362841</v>
       </c>
       <c r="D50">
-        <v>0.18637674010042429</v>
+        <v>20.23538786762472</v>
       </c>
       <c r="E50">
-        <v>28.831014380291649</v>
+        <v>26.24</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51">
-        <v>16.916112328863871</v>
+        <v>0.42121310860087952</v>
       </c>
       <c r="C51">
-        <v>18.116406844905288</v>
+        <v>0.47002217206551572</v>
       </c>
       <c r="D51">
-        <v>21.643883964936599</v>
+        <v>0.5202046175730386</v>
       </c>
       <c r="E51">
-        <v>27.948334369982561</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>1.1112997670544109</v>
+        <v>0.17264878131751199</v>
       </c>
       <c r="C52">
-        <v>1.206948111715914</v>
+        <v>0.1832873827146273</v>
       </c>
       <c r="D52">
-        <v>1.4101001811528131</v>
+        <v>0.2127504528820319</v>
       </c>
       <c r="E52">
-        <v>26.88747203559636</v>
+        <v>23.23</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>16.029834853282999</v>
+        <v>7.8491806881164444E-2</v>
       </c>
       <c r="C53">
-        <v>17.083656953362841</v>
+        <v>8.3062252281834309E-2</v>
       </c>
       <c r="D53">
-        <v>20.235387867624709</v>
+        <v>9.6669549610339092E-2</v>
       </c>
       <c r="E53">
-        <v>26.23578503979655</v>
+        <v>23.16</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54">
-        <v>16.029834853282999</v>
+        <v>0.98893082792076592</v>
       </c>
       <c r="C54">
-        <v>17.083656953362841</v>
+        <v>1.0682265194107301</v>
       </c>
       <c r="D54">
-        <v>20.235387867624709</v>
+        <v>1.216932164958481</v>
       </c>
       <c r="E54">
-        <v>26.235785039796529</v>
+        <v>23.06</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>0.42121310860087952</v>
+        <v>5.3525629475281189</v>
       </c>
       <c r="C55">
-        <v>0.47002217206551572</v>
+        <v>5.979964503625494</v>
       </c>
       <c r="D55">
-        <v>0.52020461757303871</v>
+        <v>6.5729781400834026</v>
       </c>
       <c r="E55">
-        <v>23.501526175425511</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56">
-        <v>0.17264878131751199</v>
+        <v>6.2821175470831401</v>
       </c>
       <c r="C56">
-        <v>0.1832873827146273</v>
+        <v>6.1950810823308844</v>
       </c>
       <c r="D56">
-        <v>0.21275045288203179</v>
+        <v>7.7033755830669044</v>
       </c>
       <c r="E56">
-        <v>23.22731226858205</v>
+        <v>22.62</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57">
-        <v>7.8491806881164444E-2</v>
+        <v>0.96414939807354672</v>
       </c>
       <c r="C57">
-        <v>8.3062252281834309E-2</v>
+        <v>1.015466365907542</v>
       </c>
       <c r="D57">
-        <v>9.6669549610339092E-2</v>
+        <v>1.1812613220507959</v>
       </c>
       <c r="E57">
-        <v>23.158777267919831</v>
+        <v>22.52</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>0.98893082792076614</v>
+        <v>0.60870659372981373</v>
       </c>
       <c r="C58">
-        <v>1.0682265194107301</v>
+        <v>0.64046312063339916</v>
       </c>
       <c r="D58">
-        <v>1.216932164958481</v>
+        <v>0.74555126989337517</v>
       </c>
       <c r="E58">
-        <v>23.05533719856717</v>
+        <v>22.48</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59">
-        <v>5.3525629475281189</v>
+        <v>1.329418331531335</v>
       </c>
       <c r="C59">
-        <v>5.979964503625494</v>
+        <v>1.3918571773293129</v>
       </c>
       <c r="D59">
-        <v>6.5729781400834026</v>
+        <v>1.6251130685341211</v>
       </c>
       <c r="E59">
-        <v>22.800576182273328</v>
+        <v>22.24</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>0.96414939807354683</v>
+        <v>4.1524335353631023E-2</v>
       </c>
       <c r="C60">
-        <v>1.015466365907542</v>
+        <v>4.1669835510392793E-2</v>
       </c>
       <c r="D60">
-        <v>1.181261322050795</v>
+        <v>5.0679924864135383E-2</v>
       </c>
       <c r="E60">
-        <v>22.518493960692911</v>
+        <v>22.05</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61">
-        <v>0.60870659372981351</v>
+        <v>3.218496762444131</v>
       </c>
       <c r="C61">
-        <v>0.64046312063339916</v>
+        <v>3.2853687052216469</v>
       </c>
       <c r="D61">
-        <v>0.74555126989337517</v>
+        <v>3.922056722714617</v>
       </c>
       <c r="E61">
-        <v>22.481221260485128</v>
+        <v>21.86</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62">
-        <v>130.28712015356561</v>
+        <v>1.6337898412124421E-2</v>
       </c>
       <c r="C62">
-        <v>133.12524198921091</v>
+        <v>1.649742451832235E-2</v>
       </c>
       <c r="D62">
-        <v>159.32056399618239</v>
+        <v>1.9888495276653172E-2</v>
       </c>
       <c r="E62">
-        <v>22.284201084800959</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63">
-        <v>1.329418331531335</v>
+        <v>0.46245850279519007</v>
       </c>
       <c r="C63">
-        <v>1.391857177329314</v>
+        <v>0.48383608096456399</v>
       </c>
       <c r="D63">
-        <v>1.6251130685341211</v>
+        <v>0.56168374852585379</v>
       </c>
       <c r="E63">
-        <v>22.24241459512449</v>
+        <v>21.46</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64">
-        <v>4.1524335353631023E-2</v>
+        <v>5.3161959112578323E-2</v>
       </c>
       <c r="C64">
-        <v>4.1669835510392793E-2</v>
+        <v>5.3649504777987758E-2</v>
       </c>
       <c r="D64">
-        <v>5.0679924864135383E-2</v>
+        <v>6.4536242720453246E-2</v>
       </c>
       <c r="E64">
-        <v>22.048732225412401</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65">
-        <v>3.218496762444131</v>
+        <v>8.5738989315846901</v>
       </c>
       <c r="C65">
-        <v>3.2853687052216469</v>
+        <v>8.9193065660248312</v>
       </c>
       <c r="D65">
-        <v>3.922056722714617</v>
+        <v>10.39754668636248</v>
       </c>
       <c r="E65">
-        <v>21.859893366373999</v>
+        <v>21.27</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66">
-        <v>1.6337898412124411E-2</v>
+        <v>0.1387805829606526</v>
       </c>
       <c r="C66">
-        <v>1.649742451832235E-2</v>
+        <v>0.14952001001745591</v>
       </c>
       <c r="D66">
-        <v>1.9888495276653172E-2</v>
+        <v>0.16735065683092001</v>
       </c>
       <c r="E66">
-        <v>21.73227409648873</v>
+        <v>20.59</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67">
-        <v>292.0958598115451</v>
+        <v>1.2249500713471299E-2</v>
       </c>
       <c r="C67">
-        <v>321.31720380628002</v>
+        <v>1.239954565860138E-2</v>
       </c>
       <c r="D67">
-        <v>355.44191976997229</v>
+        <v>1.4754782616624719E-2</v>
       </c>
       <c r="E67">
-        <v>21.686736675862821</v>
+        <v>20.45</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68">
-        <v>0.46245850279519002</v>
+        <v>1.6697157935548029E-2</v>
       </c>
       <c r="C68">
-        <v>0.48383608096456399</v>
+        <v>2.0236643905374559E-2</v>
       </c>
       <c r="D68">
-        <v>0.56168374852585368</v>
+        <v>2.0060850324008221E-2</v>
       </c>
       <c r="E68">
-        <v>21.45603229931481</v>
+        <v>20.149999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69">
-        <v>5.3161959112578303E-2</v>
+        <v>3.5392245096734262E-2</v>
       </c>
       <c r="C69">
-        <v>5.3649504777987737E-2</v>
+        <v>3.7458076579051813E-2</v>
       </c>
       <c r="D69">
-        <v>6.4536242720453246E-2</v>
+        <v>4.2338795273005797E-2</v>
       </c>
       <c r="E69">
-        <v>21.395531311756621</v>
+        <v>19.63</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70">
-        <v>8.5738989315846901</v>
+        <v>1.496414873744595E-2</v>
       </c>
       <c r="C70">
-        <v>8.919306566024833</v>
+        <v>1.569866110028649E-2</v>
       </c>
       <c r="D70">
-        <v>10.39754668636248</v>
+        <v>1.785465222307327E-2</v>
       </c>
       <c r="E70">
-        <v>21.2697603427514</v>
+        <v>19.32</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71">
-        <v>0.13878058296065271</v>
+        <v>4.0808649494988503</v>
       </c>
       <c r="C71">
-        <v>0.1495200100174558</v>
+        <v>4.118608762354893</v>
       </c>
       <c r="D71">
-        <v>0.16735065683092001</v>
+        <v>4.8658042151463201</v>
       </c>
       <c r="E71">
-        <v>20.5865065996787</v>
+        <v>19.23</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72">
-        <v>1.2249500713471299E-2</v>
+        <v>3.2881740914326061</v>
       </c>
       <c r="C72">
-        <v>1.239954565860138E-2</v>
+        <v>3.4800297677155259</v>
       </c>
       <c r="D72">
-        <v>1.4754782616624719E-2</v>
+        <v>3.9199496054759209</v>
       </c>
       <c r="E72">
-        <v>20.452114431066171</v>
+        <v>19.21</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73">
-        <v>229.97787653451641</v>
+        <v>5.4129324674990299E-2</v>
       </c>
       <c r="C73">
-        <v>237.60917905605839</v>
+        <v>5.2026754147497183E-2</v>
       </c>
       <c r="D73">
-        <v>276.99224851673529</v>
+        <v>4.4035330877436128E-2</v>
       </c>
       <c r="E73">
-        <v>20.442997687720101</v>
+        <v>-18.649999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74">
-        <v>360.37819025317492</v>
+        <v>9.971925330768211E-2</v>
       </c>
       <c r="C74">
-        <v>384.08658508475509</v>
+        <v>0.1007086433172347</v>
       </c>
       <c r="D74">
-        <v>433.8737260428444</v>
+        <v>0.1182363436310805</v>
       </c>
       <c r="E74">
-        <v>20.394002128163461</v>
+        <v>18.57</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75">
-        <v>1.6697157935548029E-2</v>
+        <v>1.784454154249045E-2</v>
       </c>
       <c r="C75">
-        <v>2.0236643905374559E-2</v>
+        <v>1.850806445945765E-2</v>
       </c>
       <c r="D75">
-        <v>2.0060850324008221E-2</v>
+        <v>2.115468352968353E-2</v>
       </c>
       <c r="E75">
-        <v>20.145298987074511</v>
+        <v>18.55</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76">
-        <v>3.5392245096734262E-2</v>
+        <v>10.35886910151229</v>
       </c>
       <c r="C76">
-        <v>3.745807657905182E-2</v>
+        <v>10.62738642597002</v>
       </c>
       <c r="D76">
-        <v>4.2338795273005797E-2</v>
+        <v>12.222853673511571</v>
       </c>
       <c r="E76">
-        <v>19.627322757528368</v>
+        <v>17.989999999999998</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77">
-        <v>1.496414873744595E-2</v>
+        <v>0.23258590344217281</v>
       </c>
       <c r="C77">
-        <v>1.569866110028649E-2</v>
+        <v>0.24278169821141959</v>
       </c>
       <c r="D77">
-        <v>1.7854652223073281E-2</v>
+        <v>0.2743586096217675</v>
       </c>
       <c r="E77">
-        <v>19.316190558800042</v>
+        <v>17.96</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78">
-        <v>4.0808649494988503</v>
+        <v>24.40575739836963</v>
       </c>
       <c r="C78">
-        <v>4.1186087623548921</v>
+        <v>25.313609483493391</v>
       </c>
       <c r="D78">
-        <v>4.865804215146321</v>
+        <v>28.692663615032039</v>
       </c>
       <c r="E78">
-        <v>19.234629799348419</v>
+        <v>17.57</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79">
-        <v>3.2881740914326052</v>
+        <v>17.063977864728638</v>
       </c>
       <c r="C79">
-        <v>3.4800297677155259</v>
+        <v>18.218038763201299</v>
       </c>
       <c r="D79">
-        <v>3.9199496054759222</v>
+        <v>19.928479137031761</v>
       </c>
       <c r="E79">
-        <v>19.213566449824501</v>
+        <v>16.79</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80">
-        <v>9.971925330768211E-2</v>
+        <v>12.744696588125381</v>
       </c>
       <c r="C80">
-        <v>0.1007086433172347</v>
+        <v>13.52727389334974</v>
       </c>
       <c r="D80">
-        <v>0.1182363436310805</v>
+        <v>14.875104406025461</v>
       </c>
       <c r="E80">
-        <v>18.56922280220471</v>
+        <v>16.72</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81">
-        <v>1.784454154249045E-2</v>
+        <v>21.539520038424829</v>
       </c>
       <c r="C81">
-        <v>1.850806445945765E-2</v>
+        <v>22.34508048406655</v>
       </c>
       <c r="D81">
-        <v>2.115468352968353E-2</v>
+        <v>25.137799692404961</v>
       </c>
       <c r="E81">
-        <v>18.549885292996439</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82">
-        <v>10.35886910151229</v>
+        <v>2.4355794989347621</v>
       </c>
       <c r="C82">
-        <v>10.62738642597002</v>
+        <v>2.550154556973443</v>
       </c>
       <c r="D82">
-        <v>12.222853673511571</v>
+        <v>2.841983532115111</v>
       </c>
       <c r="E82">
-        <v>17.99409331011967</v>
+        <v>16.690000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83">
-        <v>0.23258590344217281</v>
+        <v>11.254659759477869</v>
       </c>
       <c r="C83">
-        <v>0.24278169821141959</v>
+        <v>12.44550214180245</v>
       </c>
       <c r="D83">
-        <v>0.2743586096217675</v>
+        <v>13.088678557099611</v>
       </c>
       <c r="E83">
-        <v>17.960119491928079</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84">
-        <v>24.40575739836963</v>
+        <v>7.7168899312436467</v>
       </c>
       <c r="C84">
-        <v>25.31360948349338</v>
+        <v>7.7070112344260959</v>
       </c>
       <c r="D84">
-        <v>28.692663615032039</v>
+        <v>8.9677455289297381</v>
       </c>
       <c r="E84">
-        <v>17.565143120486749</v>
+        <v>16.21</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85">
-        <v>470.43646106930089</v>
+        <v>3.0002180923233548E-2</v>
       </c>
       <c r="C85">
-        <v>492.49268327680738</v>
+        <v>3.5935532754418201E-2</v>
       </c>
       <c r="D85">
-        <v>553.03378098746521</v>
+        <v>3.4826932195353252E-2</v>
       </c>
       <c r="E85">
-        <v>17.55759316155487</v>
+        <v>16.079999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86">
-        <v>17.063977864728638</v>
+        <v>0.1076279770954694</v>
       </c>
       <c r="C86">
-        <v>18.218038763201299</v>
+        <v>0.1101948734780778</v>
       </c>
       <c r="D86">
-        <v>19.928479137031768</v>
+        <v>0.1249282045203098</v>
       </c>
       <c r="E86">
-        <v>16.786831857207659</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87">
-        <v>12.744696588125381</v>
+        <v>22.132875100777579</v>
       </c>
       <c r="C87">
-        <v>13.52727389334974</v>
+        <v>24.17339829194318</v>
       </c>
       <c r="D87">
-        <v>14.875104406025461</v>
+        <v>25.6284166757851</v>
       </c>
       <c r="E87">
-        <v>16.71603402379186</v>
+        <v>15.79</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88">
-        <v>21.539520038424829</v>
+        <v>12.25334754797216</v>
       </c>
       <c r="C88">
-        <v>22.34508048406655</v>
+        <v>12.92443045182209</v>
       </c>
       <c r="D88">
-        <v>25.13779969240495</v>
+        <v>14.185665371849581</v>
       </c>
       <c r="E88">
-        <v>16.705477408786589</v>
+        <v>15.77</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89">
-        <v>21.53952003842484</v>
+        <v>7.8281493869767846</v>
       </c>
       <c r="C89">
-        <v>22.34508048406655</v>
+        <v>7.8091083999443116</v>
       </c>
       <c r="D89">
-        <v>25.13779969240495</v>
+        <v>9.0582398694240815</v>
       </c>
       <c r="E89">
-        <v>16.705477408786571</v>
+        <v>15.71</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90">
-        <v>2.435579498934763</v>
+        <v>4.6710861578547341E-2</v>
       </c>
       <c r="C90">
-        <v>2.550154556973443</v>
+        <v>4.9205769491295813E-2</v>
       </c>
       <c r="D90">
-        <v>2.841983532115111</v>
+        <v>5.3984358852779912E-2</v>
       </c>
       <c r="E90">
-        <v>16.686132945284491</v>
+        <v>15.57</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91">
-        <v>11.254659759477869</v>
+        <v>24.87882852925809</v>
       </c>
       <c r="C91">
-        <v>12.44550214180245</v>
+        <v>26.92202094851476</v>
       </c>
       <c r="D91">
-        <v>13.088678557099611</v>
+        <v>28.74087518692782</v>
       </c>
       <c r="E91">
-        <v>16.29563964452376</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92">
-        <v>7.7168899312436467</v>
+        <v>5.9803797635647484</v>
       </c>
       <c r="C92">
-        <v>7.707011234426095</v>
+        <v>6.1989408331977991</v>
       </c>
       <c r="D92">
-        <v>8.9677455289297399</v>
+        <v>6.9010320543215284</v>
       </c>
       <c r="E92">
-        <v>16.20932278198902</v>
+        <v>15.39</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93">
-        <v>7.7168899312436467</v>
+        <v>9.8184385232545317</v>
       </c>
       <c r="C93">
-        <v>7.707011234426095</v>
+        <v>9.732506503579577</v>
       </c>
       <c r="D93">
-        <v>8.9677455289297381</v>
+        <v>11.315048751983671</v>
       </c>
       <c r="E93">
-        <v>16.209322781988991</v>
+        <v>15.24</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94">
-        <v>3.0002180923233559E-2</v>
+        <v>0.1433940310101301</v>
       </c>
       <c r="C94">
-        <v>3.5935532754418208E-2</v>
+        <v>0.14817026185447241</v>
       </c>
       <c r="D94">
-        <v>3.4826932195353252E-2</v>
+        <v>0.1651282355229724</v>
       </c>
       <c r="E94">
-        <v>16.081335168482472</v>
+        <v>15.16</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95">
-        <v>0.1076279770954694</v>
+        <v>0.14302251817449191</v>
       </c>
       <c r="C95">
-        <v>0.1101948734780778</v>
+        <v>0.1494786901673899</v>
       </c>
       <c r="D95">
-        <v>0.1249282045203098</v>
+        <v>0.16435234374050159</v>
       </c>
       <c r="E95">
-        <v>16.074098846524411</v>
+        <v>14.91</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B96">
-        <v>22.132875100777579</v>
+        <v>11.917850888234019</v>
       </c>
       <c r="C96">
-        <v>24.17339829194318</v>
+        <v>12.5161233810305</v>
       </c>
       <c r="D96">
-        <v>25.6284166757851</v>
+        <v>13.68209657025446</v>
       </c>
       <c r="E96">
-        <v>15.793436501544781</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B97">
-        <v>22.132875100777579</v>
+        <v>36.78128506255829</v>
       </c>
       <c r="C97">
-        <v>24.17339829194319</v>
+        <v>39.209714134845697</v>
       </c>
       <c r="D97">
-        <v>25.62841667578509</v>
+        <v>42.124186484054903</v>
       </c>
       <c r="E97">
-        <v>15.79343650154477</v>
+        <v>14.53</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98">
-        <v>12.25334754797216</v>
+        <v>0.20313456918828429</v>
       </c>
       <c r="C98">
-        <v>12.92443045182209</v>
+        <v>0.21590938029722859</v>
       </c>
       <c r="D98">
-        <v>14.185665371849581</v>
+        <v>0.232436601074759</v>
       </c>
       <c r="E98">
-        <v>15.769713674670159</v>
+        <v>14.42</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99">
-        <v>7.8281493869767873</v>
+        <v>0.62116985356044963</v>
       </c>
       <c r="C99">
-        <v>7.8091083999443116</v>
+        <v>0.65609082664748297</v>
       </c>
       <c r="D99">
-        <v>9.0582398694240798</v>
+        <v>0.71070698228592966</v>
       </c>
       <c r="E99">
-        <v>15.71368176102667</v>
+        <v>14.41</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100">
-        <v>4.6710861578547327E-2</v>
+        <v>22.107244705218601</v>
       </c>
       <c r="C100">
-        <v>4.9205769491295813E-2</v>
+        <v>23.702081637434809</v>
       </c>
       <c r="D100">
-        <v>5.3984358852779891E-2</v>
+        <v>25.259233165262039</v>
       </c>
       <c r="E100">
-        <v>15.571319021811901</v>
+        <v>14.26</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101">
-        <v>24.878828529258101</v>
+        <v>43.22963693963694</v>
       </c>
       <c r="C101">
-        <v>26.92202094851476</v>
+        <v>46.027190307693402</v>
       </c>
       <c r="D101">
-        <v>28.74087518692782</v>
+        <v>49.388422937107137</v>
       </c>
       <c r="E101">
-        <v>15.52342648741624</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102">
-        <v>5.9803797635647484</v>
+        <v>5.110981377560325</v>
       </c>
       <c r="C102">
-        <v>6.1989408331978009</v>
+        <v>5.2992207858616531</v>
       </c>
       <c r="D102">
-        <v>6.9010320543215284</v>
+        <v>5.837174624016729</v>
       </c>
       <c r="E102">
-        <v>15.39454561674863</v>
+        <v>14.21</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103">
-        <v>0.1433940310101301</v>
+        <v>9.2933263939455876E-2</v>
       </c>
       <c r="C103">
-        <v>0.14817026185447241</v>
+        <v>8.0024967571407202E-2</v>
       </c>
       <c r="D103">
-        <v>0.16512823552297229</v>
+        <v>0.1061078284762495</v>
       </c>
       <c r="E103">
-        <v>15.15697993824222</v>
+        <v>14.18</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104">
-        <v>0.14302251817449191</v>
+        <v>1.8126352575965581</v>
       </c>
       <c r="C104">
-        <v>0.14947869016738979</v>
+        <v>1.8789146956252221</v>
       </c>
       <c r="D104">
-        <v>0.16435234374050159</v>
+        <v>2.0625715796768431</v>
       </c>
       <c r="E104">
-        <v>14.91361349125925</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105">
-        <v>11.917850888234019</v>
+        <v>17.35440245302372</v>
       </c>
       <c r="C105">
-        <v>12.5161233810305</v>
+        <v>17.450218849287211</v>
       </c>
       <c r="D105">
-        <v>13.682096570254471</v>
+        <v>19.698986488332309</v>
       </c>
       <c r="E105">
-        <v>14.803387779941209</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B106">
-        <v>11.917850888234019</v>
+        <v>0.19155932564214301</v>
       </c>
       <c r="C106">
-        <v>12.5161233810305</v>
+        <v>0.18946982918345151</v>
       </c>
       <c r="D106">
-        <v>13.68209657025446</v>
+        <v>0.21735085287716871</v>
       </c>
       <c r="E106">
-        <v>14.8033877799412</v>
+        <v>13.46</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B107">
-        <v>36.78128506255829</v>
+        <v>0.3020137654903135</v>
       </c>
       <c r="C107">
-        <v>39.209714134845719</v>
+        <v>0.32132068456418311</v>
       </c>
       <c r="D107">
-        <v>42.124186484054903</v>
+        <v>0.34086665511665509</v>
       </c>
       <c r="E107">
-        <v>14.52614124930466</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B108">
-        <v>36.78128506255829</v>
+        <v>27.356805558115148</v>
       </c>
       <c r="C108">
-        <v>39.209714134845733</v>
+        <v>28.196471179229469</v>
       </c>
       <c r="D108">
-        <v>42.124186484054903</v>
+        <v>30.82579184145763</v>
       </c>
       <c r="E108">
-        <v>14.52614124930466</v>
+        <v>12.68</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B109">
-        <v>0.20313456918828429</v>
+        <v>11.045900349580689</v>
       </c>
       <c r="C109">
-        <v>0.21590938029722859</v>
+        <v>11.627140260259459</v>
       </c>
       <c r="D109">
-        <v>0.232436601074759</v>
+        <v>12.39002778081726</v>
       </c>
       <c r="E109">
-        <v>14.42493614137865</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B110">
-        <v>0.62116985356044963</v>
+        <v>0.46567782898471749</v>
       </c>
       <c r="C110">
-        <v>0.65609082664748297</v>
+        <v>0.4882041069214445</v>
       </c>
       <c r="D110">
-        <v>0.71070698228592966</v>
+        <v>0.52153923052607254</v>
       </c>
       <c r="E110">
-        <v>14.414274648434249</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B111">
-        <v>43.22963693963694</v>
+        <v>0.15363930929333411</v>
       </c>
       <c r="C111">
-        <v>46.027190307693409</v>
+        <v>0.12397053269344289</v>
       </c>
       <c r="D111">
-        <v>49.388422937107137</v>
+        <v>0.1717840816525027</v>
       </c>
       <c r="E111">
-        <v>14.246675275274519</v>
+        <v>11.81</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B112">
-        <v>5.1109813775603241</v>
+        <v>2.706469048481432</v>
       </c>
       <c r="C112">
-        <v>5.2992207858616522</v>
+        <v>2.8388855491332281</v>
       </c>
       <c r="D112">
-        <v>5.8371746240167299</v>
+        <v>3.022901545269967</v>
       </c>
       <c r="E112">
-        <v>14.208489384147329</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B113">
-        <v>9.2933263939455876E-2</v>
+        <v>1.4839346623170151</v>
       </c>
       <c r="C113">
-        <v>8.0024967571407216E-2</v>
+        <v>1.5319587208132099</v>
       </c>
       <c r="D113">
-        <v>0.1061078284762495</v>
+        <v>1.6560174040437201</v>
       </c>
       <c r="E113">
-        <v>14.17637127797062</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114">
-        <v>1.8126352575965581</v>
+        <v>35.597808188474403</v>
       </c>
       <c r="C114">
-        <v>1.8789146956252221</v>
+        <v>36.194142050585803</v>
       </c>
       <c r="D114">
-        <v>2.0625715796768431</v>
+        <v>39.341216768492679</v>
       </c>
       <c r="E114">
-        <v>13.788561214002019</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115">
-        <v>0.19155932564214301</v>
+        <v>5.2608741727898076</v>
       </c>
       <c r="C115">
-        <v>0.18946982918345151</v>
+        <v>5.4882893459983242</v>
       </c>
       <c r="D115">
-        <v>0.21735085287716871</v>
+        <v>5.7757613889192836</v>
       </c>
       <c r="E115">
-        <v>13.463989366514831</v>
+        <v>9.7899999999999991</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116">
-        <v>0.3020137654903135</v>
+        <v>0.42761021158853968</v>
       </c>
       <c r="C116">
-        <v>0.32132068456418311</v>
+        <v>0.37775975656006622</v>
       </c>
       <c r="D116">
-        <v>0.34086665511665509</v>
+        <v>0.46656286853655282</v>
       </c>
       <c r="E116">
-        <v>12.86460885756804</v>
+        <v>9.11</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117">
-        <v>11.045900349580689</v>
+        <v>1.3381135606135609E-2</v>
       </c>
       <c r="C117">
-        <v>11.627140260259459</v>
+        <v>1.361128437451967E-2</v>
       </c>
       <c r="D117">
-        <v>12.390027780817251</v>
+        <v>1.457800209115998E-2</v>
       </c>
       <c r="E117">
-        <v>12.168563799216139</v>
+        <v>8.94</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118">
-        <v>0.46567782898471749</v>
+        <v>6.5988597606592956</v>
       </c>
       <c r="C118">
-        <v>0.48820410692144439</v>
+        <v>6.7081956001073646</v>
       </c>
       <c r="D118">
-        <v>0.52153923052607254</v>
+        <v>7.1756781072570526</v>
       </c>
       <c r="E118">
-        <v>11.995718512763521</v>
+        <v>8.74</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119">
-        <v>0.153639309293334</v>
+        <v>11.69518485274847</v>
       </c>
       <c r="C119">
-        <v>0.12397053269344289</v>
+        <v>11.06541042095968</v>
       </c>
       <c r="D119">
-        <v>0.1717840816525027</v>
+        <v>10.919126205263961</v>
       </c>
       <c r="E119">
-        <v>11.80998042924419</v>
+        <v>-6.64</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120">
-        <v>2.706469048481432</v>
+        <v>0.110353712695044</v>
       </c>
       <c r="C120">
-        <v>2.8388855491332272</v>
+        <v>0.1269978449158016</v>
       </c>
       <c r="D120">
-        <v>3.022901545269967</v>
+        <v>0.1173608831503568</v>
       </c>
       <c r="E120">
-        <v>11.69170942361529</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121">
-        <v>1.4839346623170151</v>
+        <v>4.3067626399669739E-2</v>
       </c>
       <c r="C121">
-        <v>1.5319587208132099</v>
+        <v>5.3021633369930578E-2</v>
       </c>
       <c r="D121">
-        <v>1.6560174040437201</v>
+        <v>4.557254623044097E-2</v>
       </c>
       <c r="E121">
-        <v>11.59638265056862</v>
+        <v>5.82</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B122">
-        <v>600.64666189594857</v>
+        <v>5.5221386800334161E-3</v>
       </c>
       <c r="C122">
-        <v>630.60188323609293</v>
+        <v>2.899159663865546E-3</v>
       </c>
       <c r="D122">
-        <v>666.4209307136083</v>
+        <v>5.2687809266756631E-3</v>
       </c>
       <c r="E122">
-        <v>10.950575935949169</v>
+        <v>-4.59</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123">
-        <v>335.89412644074582</v>
+        <v>45.491427152948702</v>
       </c>
       <c r="C123">
-        <v>341.87024731671579</v>
+        <v>46.473327866391898</v>
       </c>
       <c r="D123">
-        <v>370.52017938991628</v>
+        <v>47.357199710642853</v>
       </c>
       <c r="E123">
-        <v>10.30862114681211</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124">
-        <v>5.2608741727898076</v>
+        <v>0.1111498160608068</v>
       </c>
       <c r="C124">
-        <v>5.4882893459983242</v>
+        <v>0.10662771401935491</v>
       </c>
       <c r="D124">
-        <v>5.7757613889192836</v>
+        <v>0.1067205869837449</v>
       </c>
       <c r="E124">
-        <v>9.7871038009722149</v>
+        <v>-3.98</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B125">
-        <v>0.42761021158853968</v>
+        <v>2.4746403135838122</v>
       </c>
       <c r="C125">
-        <v>0.37775975656006622</v>
+        <v>2.3479773432714599</v>
       </c>
       <c r="D125">
-        <v>0.46656286853655282</v>
+        <v>2.3937450608503239</v>
       </c>
       <c r="E125">
-        <v>9.1093841756741121</v>
+        <v>-3.27</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126">
-        <v>1.3381135606135609E-2</v>
+        <v>25.63390538601146</v>
       </c>
       <c r="C126">
-        <v>1.361128437451967E-2</v>
+        <v>25.350806193059999</v>
       </c>
       <c r="D126">
-        <v>1.4578002091159991E-2</v>
+        <v>26.359539125104082</v>
       </c>
       <c r="E126">
-        <v>8.9444313267073134</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B127">
-        <v>6.5988597606592956</v>
+        <v>6.4794878201921549E-2</v>
       </c>
       <c r="C127">
-        <v>6.7081956001073646</v>
+        <v>6.3378728276948099E-2</v>
       </c>
       <c r="D127">
-        <v>7.1756781072570544</v>
+        <v>6.6031177432493218E-2</v>
       </c>
       <c r="E127">
-        <v>8.7411820756761713</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B128">
-        <v>0.1103537126950439</v>
+        <v>1.8805403724985771E-2</v>
       </c>
       <c r="C128">
-        <v>0.1269978449158016</v>
+        <v>1.8072542143285179E-2</v>
       </c>
       <c r="D128">
-        <v>0.1173608831503568</v>
+        <v>1.9146350804245541E-2</v>
       </c>
       <c r="E128">
-        <v>6.3497369360619382</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B129">
-        <v>4.3067626399669753E-2</v>
+        <v>1.9872124793641821</v>
       </c>
       <c r="C129">
-        <v>5.3021633369930578E-2</v>
+        <v>1.898764982263434</v>
       </c>
       <c r="D129">
-        <v>4.557254623044097E-2</v>
+        <v>1.956612989507726</v>
       </c>
       <c r="E129">
-        <v>5.8162477019871988</v>
+        <v>-1.54</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130">
-        <v>6.4794878201921549E-2</v>
+        <v>8.517790971289422</v>
       </c>
       <c r="C130">
-        <v>6.3378728276948085E-2</v>
+        <v>8.5721818514465582</v>
       </c>
       <c r="D130">
-        <v>6.6031177432493218E-2</v>
+        <v>8.4519369065421692</v>
       </c>
       <c r="E130">
-        <v>1.9080199930602011</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131">
-        <v>1.8805403724985771E-2</v>
+        <v>8.2788568036129959</v>
       </c>
       <c r="C131">
-        <v>1.8072542143285179E-2</v>
+        <v>8.3412027820309564</v>
       </c>
       <c r="D131">
-        <v>1.9146350804245541E-2</v>
+        <v>8.2786982833035463</v>
       </c>
       <c r="E131">
-        <v>1.8130271715824491</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B132">
-        <v>8.2788568036129959</v>
-      </c>
-      <c r="C132">
-        <v>8.3412027820309547</v>
-      </c>
-      <c r="D132">
-        <v>8.2786982833035445</v>
-      </c>
-      <c r="E132">
-        <v>-1.914760856622427E-3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B133">
-        <v>8.2788568036129959</v>
-      </c>
-      <c r="C133">
-        <v>8.3412027820309564</v>
-      </c>
-      <c r="D133">
-        <v>8.2786982833035445</v>
-      </c>
-      <c r="E133">
-        <v>-1.914760856622427E-3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B134">
-        <v>154.70628415250829</v>
-      </c>
-      <c r="C134">
-        <v>150.13587503702891</v>
-      </c>
-      <c r="D134">
-        <v>153.96808578771081</v>
-      </c>
-      <c r="E134">
-        <v>-0.4771612018486418</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B135">
-        <v>8.5177909712894238</v>
-      </c>
-      <c r="C135">
-        <v>8.5721818514465564</v>
-      </c>
-      <c r="D135">
-        <v>8.4519369065421674</v>
-      </c>
-      <c r="E135">
-        <v>-0.7731354874665034</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B136">
-        <v>1.9872124793641821</v>
-      </c>
-      <c r="C136">
-        <v>1.898764982263434</v>
-      </c>
-      <c r="D136">
-        <v>1.956612989507726</v>
-      </c>
-      <c r="E136">
-        <v>-1.539819731116328</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B137">
-        <v>2.4746403135838122</v>
-      </c>
-      <c r="C137">
-        <v>2.3479773432714608</v>
-      </c>
-      <c r="D137">
-        <v>2.3937450608503239</v>
-      </c>
-      <c r="E137">
-        <v>-3.2689701323233571</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B138">
-        <v>0.1111498160608068</v>
-      </c>
-      <c r="C138">
-        <v>0.10662771401935491</v>
-      </c>
-      <c r="D138">
-        <v>0.1067205869837449</v>
-      </c>
-      <c r="E138">
-        <v>-3.9849180448834862</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B139">
-        <v>5.5221386800334161E-3</v>
-      </c>
-      <c r="C139">
-        <v>2.899159663865546E-3</v>
-      </c>
-      <c r="D139">
-        <v>5.2687809266756631E-3</v>
-      </c>
-      <c r="E139">
-        <v>-4.5880367741184616</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B140">
-        <v>5.4129324674990313E-2</v>
-      </c>
-      <c r="C140">
-        <v>5.202675414749719E-2</v>
-      </c>
-      <c r="D140">
-        <v>4.4035330877436142E-2</v>
-      </c>
-      <c r="E140">
-        <v>-18.64792117426499</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B141">
-        <v>1.801294740923224E-2</v>
-      </c>
-      <c r="C141">
-        <v>1.6099485658309189E-2</v>
-      </c>
-      <c r="D141">
-        <v>7.8965605281394752E-3</v>
-      </c>
-      <c r="E141">
-        <v>-56.161752162268442</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modif appli evo + saison 2020/2021 SB
</commit_message>
<xml_diff>
--- a/Tableau métriques/Evolutions métriques/evo_passes.xlsx
+++ b/Tableau métriques/Evolutions métriques/evo_passes.xlsx
@@ -29,32 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00008000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFA500"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -96,15 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -530,7 +506,7 @@
       <c r="E2" t="n">
         <v>0.05440733115433372</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" t="n">
         <v>366.8139155851507</v>
       </c>
     </row>
@@ -550,7 +526,7 @@
       <c r="E3" t="n">
         <v>0.02726179371569421</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" t="n">
         <v>116.9381954112913</v>
       </c>
     </row>
@@ -574,7 +550,7 @@
       <c r="E4" t="n">
         <v>0.1464955294004714</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" t="n">
         <v>126.4121845935192</v>
       </c>
     </row>
@@ -594,7 +570,7 @@
       <c r="E5" t="n">
         <v>0.1007811998686487</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" t="n">
         <v>13.29630852966873</v>
       </c>
     </row>
@@ -618,7 +594,7 @@
       <c r="E6" t="n">
         <v>0.0348471708210419</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" t="n">
         <v>124.0122226519538</v>
       </c>
     </row>
@@ -638,7 +614,7 @@
       <c r="E7" t="n">
         <v>0.0193961707634775</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" t="n">
         <v>279.3112891277368</v>
       </c>
     </row>
@@ -662,7 +638,7 @@
       <c r="E8" t="n">
         <v>0.1406848946084119</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" t="n">
         <v>115.2757846040272</v>
       </c>
     </row>
@@ -682,7 +658,7 @@
       <c r="E9" t="n">
         <v>0.1061880785637485</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" t="n">
         <v>55.33109628400891</v>
       </c>
     </row>
@@ -706,7 +682,7 @@
       <c r="E10" t="n">
         <v>0.2098275509249417</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" t="n">
         <v>77.12816762726813</v>
       </c>
     </row>
@@ -726,7 +702,7 @@
       <c r="E11" t="n">
         <v>0.1400535902396642</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" t="n">
         <v>-9.989751107359178</v>
       </c>
     </row>
@@ -750,7 +726,7 @@
       <c r="E12" t="n">
         <v>0.009101617281544119</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" t="n">
         <v>73.98651595399734</v>
       </c>
     </row>
@@ -770,7 +746,7 @@
       <c r="E13" t="n">
         <v>0.003291963252580493</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" t="n">
         <v>-34.11898083049555</v>
       </c>
     </row>
@@ -794,7 +770,7 @@
       <c r="E14" t="n">
         <v>0.004676976802195061</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" t="n">
         <v>-56.9399929224818</v>
       </c>
     </row>
@@ -814,7 +790,7 @@
       <c r="E15" t="n">
         <v>0.009843305658093429</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" t="n">
         <v>186.6544575149587</v>
       </c>
     </row>
@@ -838,7 +814,7 @@
       <c r="E16" t="n">
         <v>0.2938442603392591</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" t="n">
         <v>53.76676337464737</v>
       </c>
     </row>
@@ -858,7 +834,7 @@
       <c r="E17" t="n">
         <v>0.1936240742216094</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" t="n">
         <v>40.24345157976518</v>
       </c>
     </row>
@@ -882,7 +858,7 @@
       <c r="E18" t="n">
         <v>0.02424292941557912</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" t="n">
         <v>48.82611543573999</v>
       </c>
     </row>
@@ -902,7 +878,7 @@
       <c r="E19" t="n">
         <v>0.02280253096359526</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" t="n">
         <v>67.61047499838745</v>
       </c>
     </row>
@@ -926,7 +902,7 @@
       <c r="E20" t="n">
         <v>0.04904470232621534</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" t="n">
         <v>-45.99078622859288</v>
       </c>
     </row>
@@ -946,7 +922,7 @@
       <c r="E21" t="n">
         <v>0.03733501329654541</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" t="n">
         <v>-4.54826546746232</v>
       </c>
     </row>
@@ -970,7 +946,7 @@
       <c r="E22" t="n">
         <v>0.01453440199611724</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" t="n">
         <v>-44.1821745430589</v>
       </c>
     </row>
@@ -990,7 +966,7 @@
       <c r="E23" t="n">
         <v>0.01941707127223067</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" t="n">
         <v>43.13121167682306</v>
       </c>
     </row>
@@ -1014,7 +990,7 @@
       <c r="E24" t="n">
         <v>0.009733215359193156</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" t="n">
         <v>-40.24828403462994</v>
       </c>
     </row>
@@ -1034,7 +1010,7 @@
       <c r="E25" t="n">
         <v>0.01965016500516979</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" t="n">
         <v>113.2888054840293</v>
       </c>
     </row>
@@ -1058,7 +1034,7 @@
       <c r="E26" t="n">
         <v>0.6018072847125094</v>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" t="n">
         <v>39.33704628947662</v>
       </c>
     </row>
@@ -1078,7 +1054,7 @@
       <c r="E27" t="n">
         <v>0.4540903808698304</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" t="n">
         <v>23.03089248740603</v>
       </c>
     </row>
@@ -1102,7 +1078,7 @@
       <c r="E28" t="n">
         <v>1.384792046834345</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" t="n">
         <v>39.04339462158168</v>
       </c>
     </row>
@@ -1122,7 +1098,7 @@
       <c r="E29" t="n">
         <v>1.106523807472647</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" t="n">
         <v>31.54082741673681</v>
       </c>
     </row>
@@ -1146,7 +1122,7 @@
       <c r="E30" t="n">
         <v>0.2138011933736385</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" t="n">
         <v>38.13425413863486</v>
       </c>
     </row>
@@ -1166,7 +1142,7 @@
       <c r="E31" t="n">
         <v>0.156551459123587</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" t="n">
         <v>17.56426622082425</v>
       </c>
     </row>
@@ -1190,7 +1166,7 @@
       <c r="E32" t="n">
         <v>1.045224750251331</v>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" t="n">
         <v>37.65473151493889</v>
       </c>
     </row>
@@ -1210,7 +1186,7 @@
       <c r="E33" t="n">
         <v>0.7723611516747285</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" t="n">
         <v>20.70470783064333</v>
       </c>
     </row>
@@ -1234,7 +1210,7 @@
       <c r="E34" t="n">
         <v>1.61344219156465</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" t="n">
         <v>35.15181304512753</v>
       </c>
     </row>
@@ -1254,7 +1230,7 @@
       <c r="E35" t="n">
         <v>1.048429101029818</v>
       </c>
-      <c r="F35" s="3" t="n">
+      <c r="F35" t="n">
         <v>27.66159976148786</v>
       </c>
     </row>
@@ -1278,7 +1254,7 @@
       <c r="E36" t="n">
         <v>1.698935457497394</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" t="n">
         <v>33.83274157994921</v>
       </c>
     </row>
@@ -1298,7 +1274,7 @@
       <c r="E37" t="n">
         <v>1.252808964338445</v>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" t="n">
         <v>44.32424167204831</v>
       </c>
     </row>
@@ -1322,7 +1298,7 @@
       <c r="E38" t="n">
         <v>21.32812673658971</v>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" t="n">
         <v>33.75366468467615</v>
       </c>
     </row>
@@ -1342,7 +1318,7 @@
       <c r="E39" t="n">
         <v>17.03898476371906</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" t="n">
         <v>26.38010437262659</v>
       </c>
     </row>
@@ -1366,7 +1342,7 @@
       <c r="E40" t="n">
         <v>7.333590469024445</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" t="n">
         <v>33.18095276421116</v>
       </c>
     </row>
@@ -1386,7 +1362,7 @@
       <c r="E41" t="n">
         <v>5.889838942150933</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" t="n">
         <v>25.50433310621904</v>
       </c>
     </row>
@@ -1410,7 +1386,7 @@
       <c r="E42" t="n">
         <v>0.03175810612589912</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F42" t="n">
         <v>32.84989284479506</v>
       </c>
     </row>
@@ -1430,7 +1406,7 @@
       <c r="E43" t="n">
         <v>0.02057164477031053</v>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F43" t="n">
         <v>40.36656386497037</v>
       </c>
     </row>
@@ -1454,7 +1430,7 @@
       <c r="E44" t="n">
         <v>2.821675977386614</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" t="n">
         <v>32.63679770417476</v>
       </c>
     </row>
@@ -1474,7 +1450,7 @@
       <c r="E45" t="n">
         <v>2.184068353895625</v>
       </c>
-      <c r="F45" s="3" t="n">
+      <c r="F45" t="n">
         <v>24.03532344210196</v>
       </c>
     </row>
@@ -1498,7 +1474,7 @@
       <c r="E46" t="n">
         <v>6.989866360792308</v>
       </c>
-      <c r="F46" s="3" t="n">
+      <c r="F46" t="n">
         <v>32.10029720952631</v>
       </c>
     </row>
@@ -1518,7 +1494,7 @@
       <c r="E47" t="n">
         <v>5.658922080954995</v>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F47" t="n">
         <v>25.2977358362552</v>
       </c>
     </row>
@@ -1542,7 +1518,7 @@
       <c r="E48" t="n">
         <v>2.628697866742415</v>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" t="n">
         <v>32.06116279646559</v>
       </c>
     </row>
@@ -1562,7 +1538,7 @@
       <c r="E49" t="n">
         <v>2.054910429706062</v>
       </c>
-      <c r="F49" s="3" t="n">
+      <c r="F49" t="n">
         <v>22.71893960268269</v>
       </c>
     </row>
@@ -1586,7 +1562,7 @@
       <c r="E50" t="n">
         <v>13.95902195019476</v>
       </c>
-      <c r="F50" s="3" t="n">
+      <c r="F50" t="n">
         <v>31.09869223512867</v>
       </c>
     </row>
@@ -1606,7 +1582,7 @@
       <c r="E51" t="n">
         <v>10.89392800510936</v>
       </c>
-      <c r="F51" s="3" t="n">
+      <c r="F51" t="n">
         <v>23.39204185674868</v>
       </c>
     </row>
@@ -1630,7 +1606,7 @@
       <c r="E52" t="n">
         <v>13.2554557219443</v>
       </c>
-      <c r="F52" s="3" t="n">
+      <c r="F52" t="n">
         <v>30.87498964680947</v>
       </c>
     </row>
@@ -1650,7 +1626,7 @@
       <c r="E53" t="n">
         <v>10.35924364016477</v>
       </c>
-      <c r="F53" s="3" t="n">
+      <c r="F53" t="n">
         <v>22.99788028152355</v>
       </c>
     </row>
@@ -1674,7 +1650,7 @@
       <c r="E54" t="n">
         <v>0.01694024287938381</v>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="F54" t="n">
         <v>30.22295372949581</v>
       </c>
     </row>
@@ -1694,7 +1670,7 @@
       <c r="E55" t="n">
         <v>0.01218805097217187</v>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" t="n">
         <v>-4.334223649899161</v>
       </c>
     </row>
@@ -1718,7 +1694,7 @@
       <c r="E56" t="n">
         <v>4.853424638830357</v>
       </c>
-      <c r="F56" s="3" t="n">
+      <c r="F56" t="n">
         <v>29.17485878144494</v>
       </c>
     </row>
@@ -1738,7 +1714,7 @@
       <c r="E57" t="n">
         <v>3.878197156005868</v>
       </c>
-      <c r="F57" s="3" t="n">
+      <c r="F57" t="n">
         <v>38.21591571789303</v>
       </c>
     </row>
@@ -1762,7 +1738,7 @@
       <c r="E58" t="n">
         <v>4.771598382848934</v>
       </c>
-      <c r="F58" s="3" t="n">
+      <c r="F58" t="n">
         <v>28.9349027121342</v>
       </c>
     </row>
@@ -1782,7 +1758,7 @@
       <c r="E59" t="n">
         <v>3.811898489620148</v>
       </c>
-      <c r="F59" s="3" t="n">
+      <c r="F59" t="n">
         <v>38.54960596903221</v>
       </c>
     </row>
@@ -1806,7 +1782,7 @@
       <c r="E60" t="n">
         <v>0.09678484323833444</v>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" t="n">
         <v>28.50624252874552</v>
       </c>
     </row>
@@ -1826,7 +1802,7 @@
       <c r="E61" t="n">
         <v>0.0727098713935805</v>
       </c>
-      <c r="F61" s="3" t="n">
+      <c r="F61" t="n">
         <v>41.78844180376205</v>
       </c>
     </row>
@@ -1850,7 +1826,7 @@
       <c r="E62" t="n">
         <v>0.0338348442941835</v>
       </c>
-      <c r="F62" s="2" t="n">
+      <c r="F62" t="n">
         <v>-27.37460630619178</v>
       </c>
     </row>
@@ -1870,7 +1846,7 @@
       <c r="E63" t="n">
         <v>0.0436434378504898</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" t="n">
         <v>81.70989698264836</v>
       </c>
     </row>
@@ -1894,7 +1870,7 @@
       <c r="E64" t="n">
         <v>0.02252053952446486</v>
       </c>
-      <c r="F64" s="3" t="n">
+      <c r="F64" t="n">
         <v>27.37087375895347</v>
       </c>
     </row>
@@ -1914,7 +1890,7 @@
       <c r="E65" t="n">
         <v>0.01590799568389823</v>
       </c>
-      <c r="F65" s="4" t="n">
+      <c r="F65" t="n">
         <v>-12.15944424486189</v>
       </c>
     </row>
@@ -1938,7 +1914,7 @@
       <c r="E66" t="n">
         <v>0.5059034380208655</v>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" t="n">
         <v>26.56630689538418</v>
       </c>
     </row>
@@ -1958,7 +1934,7 @@
       <c r="E67" t="n">
         <v>0.350070008451128</v>
       </c>
-      <c r="F67" s="3" t="n">
+      <c r="F67" t="n">
         <v>51.9878032559194</v>
       </c>
     </row>
@@ -1982,7 +1958,7 @@
       <c r="E68" t="n">
         <v>2.260769928723366</v>
       </c>
-      <c r="F68" s="2" t="n">
+      <c r="F68" t="n">
         <v>26.03873609557121</v>
       </c>
     </row>
@@ -2002,7 +1978,7 @@
       <c r="E69" t="n">
         <v>1.652039848570829</v>
       </c>
-      <c r="F69" s="3" t="n">
+      <c r="F69" t="n">
         <v>26.76855001066064</v>
       </c>
     </row>
@@ -2026,7 +2002,7 @@
       <c r="E70" t="n">
         <v>1.500884732557371</v>
       </c>
-      <c r="F70" s="2" t="n">
+      <c r="F70" t="n">
         <v>22.54151303606669</v>
       </c>
     </row>
@@ -2046,7 +2022,7 @@
       <c r="E71" t="n">
         <v>1.206417262015781</v>
       </c>
-      <c r="F71" s="3" t="n">
+      <c r="F71" t="n">
         <v>27.50934222311263</v>
       </c>
     </row>
@@ -2070,7 +2046,7 @@
       <c r="E72" t="n">
         <v>0.26101318088745</v>
       </c>
-      <c r="F72" s="2" t="n">
+      <c r="F72" t="n">
         <v>22.22832150696652</v>
       </c>
     </row>
@@ -2090,7 +2066,7 @@
       <c r="E73" t="n">
         <v>0.1966114983804183</v>
       </c>
-      <c r="F73" s="3" t="n">
+      <c r="F73" t="n">
         <v>28.14013402402314</v>
       </c>
     </row>
@@ -2114,7 +2090,7 @@
       <c r="E74" t="n">
         <v>9.314058915204189</v>
       </c>
-      <c r="F74" s="2" t="n">
+      <c r="F74" t="n">
         <v>21.55580258340185</v>
       </c>
     </row>
@@ -2134,7 +2110,7 @@
       <c r="E75" t="n">
         <v>6.313280751009366</v>
       </c>
-      <c r="F75" s="3" t="n">
+      <c r="F75" t="n">
         <v>15.78727175061729</v>
       </c>
     </row>
@@ -2158,7 +2134,7 @@
       <c r="E76" t="n">
         <v>0.6767668553589014</v>
       </c>
-      <c r="F76" s="2" t="n">
+      <c r="F76" t="n">
         <v>21.50198556856009</v>
       </c>
     </row>
@@ -2178,7 +2154,7 @@
       <c r="E77" t="n">
         <v>0.4620334863862079</v>
       </c>
-      <c r="F77" s="3" t="n">
+      <c r="F77" t="n">
         <v>13.99761075722366</v>
       </c>
     </row>
@@ -2202,7 +2178,7 @@
       <c r="E78" t="n">
         <v>0.04532404202502678</v>
       </c>
-      <c r="F78" s="2" t="n">
+      <c r="F78" t="n">
         <v>20.3141523123506</v>
       </c>
     </row>
@@ -2222,7 +2198,7 @@
       <c r="E79" t="n">
         <v>0.03282445289590195</v>
       </c>
-      <c r="F79" s="3" t="n">
+      <c r="F79" t="n">
         <v>39.69679126433446</v>
       </c>
     </row>
@@ -2246,7 +2222,7 @@
       <c r="E80" t="n">
         <v>0.2916978700239132</v>
       </c>
-      <c r="F80" s="2" t="n">
+      <c r="F80" t="n">
         <v>19.07512509511173</v>
       </c>
     </row>
@@ -2266,7 +2242,7 @@
       <c r="E81" t="n">
         <v>0.2242887598444029</v>
       </c>
-      <c r="F81" s="3" t="n">
+      <c r="F81" t="n">
         <v>43.76764617968875</v>
       </c>
     </row>
@@ -2290,7 +2266,7 @@
       <c r="E82" t="n">
         <v>0.7874350047722007</v>
       </c>
-      <c r="F82" s="2" t="n">
+      <c r="F82" t="n">
         <v>18.43305120220163</v>
       </c>
     </row>
@@ -2310,7 +2286,7 @@
       <c r="E83" t="n">
         <v>0.5616293101307946</v>
       </c>
-      <c r="F83" s="3" t="n">
+      <c r="F83" t="n">
         <v>42.25010746572876</v>
       </c>
     </row>
@@ -2334,7 +2310,7 @@
       <c r="E84" t="n">
         <v>7.016562263564377</v>
       </c>
-      <c r="F84" s="3" t="n">
+      <c r="F84" t="n">
         <v>17.21631571245998</v>
       </c>
     </row>
@@ -2354,7 +2330,7 @@
       <c r="E85" t="n">
         <v>5.700365708380979</v>
       </c>
-      <c r="F85" s="3" t="n">
+      <c r="F85" t="n">
         <v>17.32201768575619</v>
       </c>
     </row>
@@ -2378,7 +2354,7 @@
       <c r="E86" t="n">
         <v>1.305199128245488</v>
       </c>
-      <c r="F86" s="3" t="n">
+      <c r="F86" t="n">
         <v>17.01525270639302</v>
       </c>
     </row>
@@ -2398,7 +2374,7 @@
       <c r="E87" t="n">
         <v>1.052535566619967</v>
       </c>
-      <c r="F87" s="3" t="n">
+      <c r="F87" t="n">
         <v>18.00279275413004</v>
       </c>
     </row>
@@ -2422,7 +2398,7 @@
       <c r="E88" t="n">
         <v>0.4630520120463925</v>
       </c>
-      <c r="F88" s="2" t="n">
+      <c r="F88" t="n">
         <v>-16.95610605404492</v>
       </c>
     </row>
@@ -2442,7 +2418,7 @@
       <c r="E89" t="n">
         <v>0.4798557632528493</v>
       </c>
-      <c r="F89" s="3" t="n">
+      <c r="F89" t="n">
         <v>34.37017584832935</v>
       </c>
     </row>
@@ -2466,7 +2442,7 @@
       <c r="E90" t="n">
         <v>0.05479884269304456</v>
       </c>
-      <c r="F90" s="2" t="n">
+      <c r="F90" t="n">
         <v>16.04191705821724</v>
       </c>
     </row>
@@ -2486,7 +2462,7 @@
       <c r="E91" t="n">
         <v>0.02441658913301864</v>
       </c>
-      <c r="F91" s="5" t="n">
+      <c r="F91" t="n">
         <v>6.799596576380073</v>
       </c>
     </row>
@@ -2510,7 +2486,7 @@
       <c r="E92" t="n">
         <v>12.42227489097752</v>
       </c>
-      <c r="F92" s="2" t="n">
+      <c r="F92" t="n">
         <v>15.47982793581621</v>
       </c>
     </row>
@@ -2530,7 +2506,7 @@
       <c r="E93" t="n">
         <v>9.699634972805423</v>
       </c>
-      <c r="F93" s="3" t="n">
+      <c r="F93" t="n">
         <v>7.736229279552174</v>
       </c>
     </row>
@@ -2554,7 +2530,7 @@
       <c r="E94" t="n">
         <v>0.1028335935842741</v>
       </c>
-      <c r="F94" s="2" t="n">
+      <c r="F94" t="n">
         <v>15.31318523283398</v>
       </c>
     </row>
@@ -2574,7 +2550,7 @@
       <c r="E95" t="n">
         <v>0.08391804856716703</v>
       </c>
-      <c r="F95" s="3" t="n">
+      <c r="F95" t="n">
         <v>18.4875288090719</v>
       </c>
     </row>
@@ -2598,7 +2574,7 @@
       <c r="E96" t="n">
         <v>0.5662598198252325</v>
       </c>
-      <c r="F96" s="2" t="n">
+      <c r="F96" t="n">
         <v>15.13714972370172</v>
       </c>
     </row>
@@ -2618,7 +2594,7 @@
       <c r="E97" t="n">
         <v>0.3813153633263957</v>
       </c>
-      <c r="F97" s="2" t="n">
+      <c r="F97" t="n">
         <v>-1.012503005580881</v>
       </c>
     </row>
@@ -2642,7 +2618,7 @@
       <c r="E98" t="n">
         <v>0.05784666282952412</v>
       </c>
-      <c r="F98" s="2" t="n">
+      <c r="F98" t="n">
         <v>14.71074191560542</v>
       </c>
     </row>
@@ -2662,7 +2638,7 @@
       <c r="E99" t="n">
         <v>0.04271078380667202</v>
       </c>
-      <c r="F99" s="3" t="n">
+      <c r="F99" t="n">
         <v>17.76145274112977</v>
       </c>
     </row>
@@ -2686,7 +2662,7 @@
       <c r="E100" t="n">
         <v>0.1322271641155611</v>
       </c>
-      <c r="F100" s="2" t="n">
+      <c r="F100" t="n">
         <v>13.61259466228174</v>
       </c>
     </row>
@@ -2706,7 +2682,7 @@
       <c r="E101" t="n">
         <v>0.1086355576305335</v>
       </c>
-      <c r="F101" s="3" t="n">
+      <c r="F101" t="n">
         <v>9.562387237618674</v>
       </c>
     </row>
@@ -2730,7 +2706,7 @@
       <c r="E102" t="n">
         <v>4.231394293427466</v>
       </c>
-      <c r="F102" s="2" t="n">
+      <c r="F102" t="n">
         <v>13.47878120829422</v>
       </c>
     </row>
@@ -2750,7 +2726,7 @@
       <c r="E103" t="n">
         <v>3.379995836444955</v>
       </c>
-      <c r="F103" s="3" t="n">
+      <c r="F103" t="n">
         <v>13.84509966767828</v>
       </c>
     </row>
@@ -2774,7 +2750,7 @@
       <c r="E104" t="n">
         <v>1.793111225728084</v>
       </c>
-      <c r="F104" s="2" t="n">
+      <c r="F104" t="n">
         <v>13.40867248059079</v>
       </c>
     </row>
@@ -2794,7 +2770,7 @@
       <c r="E105" t="n">
         <v>1.426032459353403</v>
       </c>
-      <c r="F105" s="5" t="n">
+      <c r="F105" t="n">
         <v>3.801520211481798</v>
       </c>
     </row>
@@ -2818,7 +2794,7 @@
       <c r="E106" t="n">
         <v>0.8368069348030375</v>
       </c>
-      <c r="F106" s="2" t="n">
+      <c r="F106" t="n">
         <v>13.40181691407203</v>
       </c>
     </row>
@@ -2838,7 +2814,7 @@
       <c r="E107" t="n">
         <v>0.6344636383965176</v>
       </c>
-      <c r="F107" s="3" t="n">
+      <c r="F107" t="n">
         <v>18.94704941091557</v>
       </c>
     </row>
@@ -2862,7 +2838,7 @@
       <c r="E108" t="n">
         <v>0.06032675866872172</v>
       </c>
-      <c r="F108" s="2" t="n">
+      <c r="F108" t="n">
         <v>-12.70772219758293</v>
       </c>
     </row>
@@ -2882,7 +2858,7 @@
       <c r="E109" t="n">
         <v>0.03591848495263986</v>
       </c>
-      <c r="F109" s="5" t="n">
+      <c r="F109" t="n">
         <v>9.592235900073224</v>
       </c>
     </row>
@@ -2906,7 +2882,7 @@
       <c r="E110" t="n">
         <v>13.6612360287811</v>
       </c>
-      <c r="F110" s="3" t="n">
+      <c r="F110" t="n">
         <v>12.23367829528377</v>
       </c>
     </row>
@@ -2926,7 +2902,7 @@
       <c r="E111" t="n">
         <v>11.45856890573449</v>
       </c>
-      <c r="F111" s="5" t="n">
+      <c r="F111" t="n">
         <v>10.60814691124492</v>
       </c>
     </row>
@@ -2950,7 +2926,7 @@
       <c r="E112" t="n">
         <v>0.01974638291031754</v>
       </c>
-      <c r="F112" s="3" t="n">
+      <c r="F112" t="n">
         <v>12.07767169838055</v>
       </c>
     </row>
@@ -2970,7 +2946,7 @@
       <c r="E113" t="n">
         <v>0.01773340344221607</v>
       </c>
-      <c r="F113" s="2" t="n">
+      <c r="F113" t="n">
         <v>18.13226812159846</v>
       </c>
     </row>
@@ -2994,7 +2970,7 @@
       <c r="E114" t="n">
         <v>0.01417045326785669</v>
       </c>
-      <c r="F114" s="5" t="n">
+      <c r="F114" t="n">
         <v>-12.06305817649614</v>
       </c>
     </row>
@@ -3014,7 +2990,7 @@
       <c r="E115" t="n">
         <v>0.004813531327742332</v>
       </c>
-      <c r="F115" s="4" t="n">
+      <c r="F115" t="n">
         <v>-72.05710703674634</v>
       </c>
     </row>
@@ -3038,7 +3014,7 @@
       <c r="E116" t="n">
         <v>0.1428016396753781</v>
       </c>
-      <c r="F116" s="2" t="n">
+      <c r="F116" t="n">
         <v>12.01305765147026</v>
       </c>
     </row>
@@ -3058,7 +3034,7 @@
       <c r="E117" t="n">
         <v>0.08299573806984956</v>
       </c>
-      <c r="F117" s="4" t="n">
+      <c r="F117" t="n">
         <v>-18.2957472719848</v>
       </c>
     </row>
@@ -3082,7 +3058,7 @@
       <c r="E118" t="n">
         <v>1.635194822477348</v>
       </c>
-      <c r="F118" s="2" t="n">
+      <c r="F118" t="n">
         <v>11.87000010843891</v>
       </c>
     </row>
@@ -3102,7 +3078,7 @@
       <c r="E119" t="n">
         <v>1.440486758322611</v>
       </c>
-      <c r="F119" s="3" t="n">
+      <c r="F119" t="n">
         <v>18.29450329019944</v>
       </c>
     </row>
@@ -3126,7 +3102,7 @@
       <c r="E120" t="n">
         <v>0.008474428004029663</v>
       </c>
-      <c r="F120" s="2" t="n">
+      <c r="F120" t="n">
         <v>11.68663712607986</v>
       </c>
     </row>
@@ -3146,7 +3122,7 @@
       <c r="E121" t="n">
         <v>0.007615893009322492</v>
       </c>
-      <c r="F121" s="3" t="n">
+      <c r="F121" t="n">
         <v>67.88365593903494</v>
       </c>
     </row>
@@ -3170,7 +3146,7 @@
       <c r="E122" t="n">
         <v>10.45890925913629</v>
       </c>
-      <c r="F122" s="2" t="n">
+      <c r="F122" t="n">
         <v>11.60076821486816</v>
       </c>
     </row>
@@ -3190,7 +3166,7 @@
       <c r="E123" t="n">
         <v>9.235035460643852</v>
       </c>
-      <c r="F123" s="3" t="n">
+      <c r="F123" t="n">
         <v>17.35003980338496</v>
       </c>
     </row>
@@ -3214,7 +3190,7 @@
       <c r="E124" t="n">
         <v>0.02417722260772849</v>
       </c>
-      <c r="F124" s="2" t="n">
+      <c r="F124" t="n">
         <v>11.42933626066623</v>
       </c>
     </row>
@@ -3234,7 +3210,7 @@
       <c r="E125" t="n">
         <v>0.02129354236854769</v>
       </c>
-      <c r="F125" s="5" t="n">
+      <c r="F125" t="n">
         <v>79.10640227130095</v>
       </c>
     </row>
@@ -3258,7 +3234,7 @@
       <c r="E126" t="n">
         <v>0.009681080166954164</v>
       </c>
-      <c r="F126" s="5" t="n">
+      <c r="F126" t="n">
         <v>-10.8681958158489</v>
       </c>
     </row>
@@ -3278,7 +3254,7 @@
       <c r="E127" t="n">
         <v>0.01137675400005241</v>
       </c>
-      <c r="F127" s="3" t="n">
+      <c r="F127" t="n">
         <v>231.3111834015554</v>
       </c>
     </row>
@@ -3302,7 +3278,7 @@
       <c r="E128" t="n">
         <v>12.25376011089718</v>
       </c>
-      <c r="F128" s="2" t="n">
+      <c r="F128" t="n">
         <v>10.853923632269</v>
       </c>
     </row>
@@ -3322,7 +3298,7 @@
       <c r="E129" t="n">
         <v>10.86874796549616</v>
       </c>
-      <c r="F129" s="3" t="n">
+      <c r="F129" t="n">
         <v>13.1685703926567</v>
       </c>
     </row>
@@ -3346,7 +3322,7 @@
       <c r="E130" t="n">
         <v>0.07101292346687334</v>
       </c>
-      <c r="F130" s="2" t="n">
+      <c r="F130" t="n">
         <v>10.80031714102586</v>
       </c>
     </row>
@@ -3366,7 +3342,7 @@
       <c r="E131" t="n">
         <v>0.05530925588668963</v>
       </c>
-      <c r="F131" s="3" t="n">
+      <c r="F131" t="n">
         <v>18.35792643221201</v>
       </c>
     </row>
@@ -3390,7 +3366,7 @@
       <c r="E132" t="n">
         <v>0.2855189212223725</v>
       </c>
-      <c r="F132" s="2" t="n">
+      <c r="F132" t="n">
         <v>10.70759450147811</v>
       </c>
     </row>
@@ -3410,7 +3386,7 @@
       <c r="E133" t="n">
         <v>0.2401905026979526</v>
       </c>
-      <c r="F133" s="3" t="n">
+      <c r="F133" t="n">
         <v>13.0979769819223</v>
       </c>
     </row>
@@ -3434,7 +3410,7 @@
       <c r="E134" t="n">
         <v>0.003195084645801379</v>
       </c>
-      <c r="F134" s="2" t="n">
+      <c r="F134" t="n">
         <v>-10.27275347498774</v>
       </c>
     </row>
@@ -3454,7 +3430,7 @@
       <c r="E135" t="n">
         <v>0.002860072667841498</v>
       </c>
-      <c r="F135" s="3" t="n">
+      <c r="F135" t="n">
         <v>71.49368486732013</v>
       </c>
     </row>
@@ -3478,7 +3454,7 @@
       <c r="E136" t="n">
         <v>27.01939638184125</v>
       </c>
-      <c r="F136" s="3" t="n">
+      <c r="F136" t="n">
         <v>10.12166527567636</v>
       </c>
     </row>
@@ -3498,7 +3474,7 @@
       <c r="E137" t="n">
         <v>22.34762159092938</v>
       </c>
-      <c r="F137" s="5" t="n">
+      <c r="F137" t="n">
         <v>10.57304140588094</v>
       </c>
     </row>
@@ -3522,7 +3498,7 @@
       <c r="E138" t="n">
         <v>30.28973920426278</v>
       </c>
-      <c r="F138" s="2" t="n">
+      <c r="F138" t="n">
         <v>9.935431723454158</v>
       </c>
     </row>
@@ -3542,7 +3518,7 @@
       <c r="E139" t="n">
         <v>25.06189079883052</v>
       </c>
-      <c r="F139" s="5" t="n">
+      <c r="F139" t="n">
         <v>10.32556895164031</v>
       </c>
     </row>
@@ -3566,7 +3542,7 @@
       <c r="E140" t="n">
         <v>4.290887939932896</v>
       </c>
-      <c r="F140" s="2" t="n">
+      <c r="F140" t="n">
         <v>9.854147821574049</v>
       </c>
     </row>
@@ -3586,7 +3562,7 @@
       <c r="E141" t="n">
         <v>3.878061660020994</v>
       </c>
-      <c r="F141" s="3" t="n">
+      <c r="F141" t="n">
         <v>57.7247048998565</v>
       </c>
     </row>
@@ -3610,7 +3586,7 @@
       <c r="E142" t="n">
         <v>4.44749804412473</v>
       </c>
-      <c r="F142" s="2" t="n">
+      <c r="F142" t="n">
         <v>8.867353266896824</v>
       </c>
     </row>
@@ -3630,7 +3606,7 @@
       <c r="E143" t="n">
         <v>4.053070815457162</v>
       </c>
-      <c r="F143" s="3" t="n">
+      <c r="F143" t="n">
         <v>57.67637892922873</v>
       </c>
     </row>
@@ -3654,7 +3630,7 @@
       <c r="E144" t="n">
         <v>2.9960167386073</v>
       </c>
-      <c r="F144" s="2" t="n">
+      <c r="F144" t="n">
         <v>8.217438061549068</v>
       </c>
     </row>
@@ -3674,7 +3650,7 @@
       <c r="E145" t="n">
         <v>2.477476803414239</v>
       </c>
-      <c r="F145" s="3" t="n">
+      <c r="F145" t="n">
         <v>12.5873019274757</v>
       </c>
     </row>
@@ -3698,7 +3674,7 @@
       <c r="E146" t="n">
         <v>0.1764726916453925</v>
       </c>
-      <c r="F146" s="2" t="n">
+      <c r="F146" t="n">
         <v>8.097872881988666</v>
       </c>
     </row>
@@ -3718,7 +3694,7 @@
       <c r="E147" t="n">
         <v>0.1457576851533093</v>
       </c>
-      <c r="F147" s="3" t="n">
+      <c r="F147" t="n">
         <v>18.0688552449257</v>
       </c>
     </row>
@@ -3742,7 +3718,7 @@
       <c r="E148" t="n">
         <v>2.666787497954636</v>
       </c>
-      <c r="F148" s="2" t="n">
+      <c r="F148" t="n">
         <v>7.990685648356552</v>
       </c>
     </row>
@@ -3762,7 +3738,7 @@
       <c r="E149" t="n">
         <v>2.037877907679336</v>
       </c>
-      <c r="F149" s="4" t="n">
+      <c r="F149" t="n">
         <v>-13.20808616907792</v>
       </c>
     </row>
@@ -3786,7 +3762,7 @@
       <c r="E150" t="n">
         <v>14.85361220058565</v>
       </c>
-      <c r="F150" s="2" t="n">
+      <c r="F150" t="n">
         <v>7.966847354351014</v>
       </c>
     </row>
@@ -3806,7 +3782,7 @@
       <c r="E151" t="n">
         <v>13.24661362716271</v>
       </c>
-      <c r="F151" s="3" t="n">
+      <c r="F151" t="n">
         <v>12.57456053258193</v>
       </c>
     </row>
@@ -3830,7 +3806,7 @@
       <c r="E152" t="n">
         <v>2.200532393939806</v>
       </c>
-      <c r="F152" s="2" t="n">
+      <c r="F152" t="n">
         <v>7.959869744920256</v>
       </c>
     </row>
@@ -3850,7 +3826,7 @@
       <c r="E153" t="n">
         <v>1.659162727207865</v>
       </c>
-      <c r="F153" s="4" t="n">
+      <c r="F153" t="n">
         <v>-11.26875448630932</v>
       </c>
     </row>
@@ -3874,7 +3850,7 @@
       <c r="E154" t="n">
         <v>0.04378461166333792</v>
       </c>
-      <c r="F154" s="3" t="n">
+      <c r="F154" t="n">
         <v>7.918080831290951</v>
       </c>
     </row>
@@ -3894,7 +3870,7 @@
       <c r="E155" t="n">
         <v>0.03718255607203978</v>
       </c>
-      <c r="F155" s="3" t="n">
+      <c r="F155" t="n">
         <v>16.49834430188186</v>
       </c>
     </row>
@@ -3918,7 +3894,7 @@
       <c r="E156" t="n">
         <v>0.7593091324361677</v>
       </c>
-      <c r="F156" s="2" t="n">
+      <c r="F156" t="n">
         <v>7.861991786335153</v>
       </c>
     </row>
@@ -3938,7 +3914,7 @@
       <c r="E157" t="n">
         <v>0.6161018831311666</v>
       </c>
-      <c r="F157" s="5" t="n">
+      <c r="F157" t="n">
         <v>9.478666589476404</v>
       </c>
     </row>
@@ -3962,7 +3938,7 @@
       <c r="E158" t="n">
         <v>8.797423404074525</v>
       </c>
-      <c r="F158" s="2" t="n">
+      <c r="F158" t="n">
         <v>7.838055161859247</v>
       </c>
     </row>
@@ -3982,7 +3958,7 @@
       <c r="E159" t="n">
         <v>6.885848342386259</v>
       </c>
-      <c r="F159" s="3" t="n">
+      <c r="F159" t="n">
         <v>31.5155137238872</v>
       </c>
     </row>
@@ -4006,7 +3982,7 @@
       <c r="E160" t="n">
         <v>8.776833328060722</v>
       </c>
-      <c r="F160" s="2" t="n">
+      <c r="F160" t="n">
         <v>-7.669175672436842</v>
       </c>
     </row>
@@ -4026,7 +4002,7 @@
       <c r="E161" t="n">
         <v>8.15679794657391</v>
       </c>
-      <c r="F161" s="3" t="n">
+      <c r="F161" t="n">
         <v>19.06470685898059</v>
       </c>
     </row>
@@ -4050,7 +4026,7 @@
       <c r="E162" t="n">
         <v>8.663906114277674</v>
       </c>
-      <c r="F162" s="2" t="n">
+      <c r="F162" t="n">
         <v>-7.530623921244416</v>
       </c>
     </row>
@@ -4070,7 +4046,7 @@
       <c r="E163" t="n">
         <v>8.08373302874541</v>
       </c>
-      <c r="F163" s="3" t="n">
+      <c r="F163" t="n">
         <v>19.7217822675696</v>
       </c>
     </row>
@@ -4094,7 +4070,7 @@
       <c r="E164" t="n">
         <v>9.431094624411395</v>
       </c>
-      <c r="F164" s="2" t="n">
+      <c r="F164" t="n">
         <v>7.49169181191477</v>
       </c>
     </row>
@@ -4114,7 +4090,7 @@
       <c r="E165" t="n">
         <v>7.662187983858598</v>
       </c>
-      <c r="F165" s="3" t="n">
+      <c r="F165" t="n">
         <v>30.62338584391828</v>
       </c>
     </row>
@@ -4138,7 +4114,7 @@
       <c r="E166" t="n">
         <v>25.65198252265822</v>
       </c>
-      <c r="F166" s="3" t="n">
+      <c r="F166" t="n">
         <v>7.385976174647931</v>
       </c>
     </row>
@@ -4158,7 +4134,7 @@
       <c r="E167" t="n">
         <v>22.36325089398123</v>
       </c>
-      <c r="F167" s="5" t="n">
+      <c r="F167" t="n">
         <v>8.458461358250029</v>
       </c>
     </row>
@@ -4182,7 +4158,7 @@
       <c r="E168" t="n">
         <v>27.62915079479133</v>
       </c>
-      <c r="F168" s="2" t="n">
+      <c r="F168" t="n">
         <v>7.343316397819919</v>
       </c>
     </row>
@@ -4202,7 +4178,7 @@
       <c r="E169" t="n">
         <v>25.87666532914726</v>
       </c>
-      <c r="F169" s="3" t="n">
+      <c r="F169" t="n">
         <v>13.80757837929137</v>
       </c>
     </row>
@@ -4226,7 +4202,7 @@
       <c r="E170" t="n">
         <v>19.27242142150217</v>
       </c>
-      <c r="F170" s="2" t="n">
+      <c r="F170" t="n">
         <v>7.122670644463864</v>
       </c>
     </row>
@@ -4246,7 +4222,7 @@
       <c r="E171" t="n">
         <v>17.95574378776538</v>
       </c>
-      <c r="F171" s="3" t="n">
+      <c r="F171" t="n">
         <v>12.82265266411069</v>
       </c>
     </row>
@@ -4270,7 +4246,7 @@
       <c r="E172" t="n">
         <v>1.4481798824113</v>
       </c>
-      <c r="F172" s="3" t="n">
+      <c r="F172" t="n">
         <v>6.953163837057894</v>
       </c>
     </row>
@@ -4290,7 +4266,7 @@
       <c r="E173" t="n">
         <v>1.244326231275183</v>
       </c>
-      <c r="F173" s="3" t="n">
+      <c r="F173" t="n">
         <v>27.7644489424538</v>
       </c>
     </row>
@@ -4314,7 +4290,7 @@
       <c r="E174" t="n">
         <v>9.068499284389691</v>
       </c>
-      <c r="F174" s="2" t="n">
+      <c r="F174" t="n">
         <v>6.69547220464873</v>
       </c>
     </row>
@@ -4334,7 +4310,7 @@
       <c r="E175" t="n">
         <v>8.704671582575195</v>
       </c>
-      <c r="F175" s="3" t="n">
+      <c r="F175" t="n">
         <v>57.08402022674218</v>
       </c>
     </row>
@@ -4358,7 +4334,7 @@
       <c r="E176" t="n">
         <v>0.002757234475521053</v>
       </c>
-      <c r="F176" s="4" t="n">
+      <c r="F176" t="n">
         <v>-6.576619170763101</v>
       </c>
     </row>
@@ -4378,7 +4354,7 @@
       <c r="E177" t="n">
         <v>0.002517963436371748</v>
       </c>
-      <c r="F177" s="3" t="n">
+      <c r="F177" t="n">
         <v>75.13108021817307</v>
       </c>
     </row>
@@ -4402,7 +4378,7 @@
       <c r="E178" t="n">
         <v>0.2134497534786503</v>
       </c>
-      <c r="F178" s="2" t="n">
+      <c r="F178" t="n">
         <v>-6.528626897216494</v>
       </c>
     </row>
@@ -4422,7 +4398,7 @@
       <c r="E179" t="n">
         <v>0.1882951873893342</v>
       </c>
-      <c r="F179" s="3" t="n">
+      <c r="F179" t="n">
         <v>29.93979923374469</v>
       </c>
     </row>
@@ -4446,7 +4422,7 @@
       <c r="E180" t="n">
         <v>26.75044556164211</v>
       </c>
-      <c r="F180" s="2" t="n">
+      <c r="F180" t="n">
         <v>-6.507531807575975</v>
       </c>
     </row>
@@ -4466,7 +4442,7 @@
       <c r="E181" t="n">
         <v>23.32865074863571</v>
       </c>
-      <c r="F181" s="5" t="n">
+      <c r="F181" t="n">
         <v>-2.858118441515422</v>
       </c>
     </row>
@@ -4490,7 +4466,7 @@
       <c r="E182" t="n">
         <v>7.190488044706361</v>
       </c>
-      <c r="F182" s="2" t="n">
+      <c r="F182" t="n">
         <v>-6.460809256832593</v>
       </c>
     </row>
@@ -4510,7 +4486,7 @@
       <c r="E183" t="n">
         <v>6.377980956418208</v>
       </c>
-      <c r="F183" s="5" t="n">
+      <c r="F183" t="n">
         <v>7.93525642425743</v>
       </c>
     </row>
@@ -4534,7 +4510,7 @@
       <c r="E184" t="n">
         <v>1.212384235703445</v>
       </c>
-      <c r="F184" s="2" t="n">
+      <c r="F184" t="n">
         <v>6.446163898995021</v>
       </c>
     </row>
@@ -4554,7 +4530,7 @@
       <c r="E185" t="n">
         <v>1.039094452279696</v>
       </c>
-      <c r="F185" s="3" t="n">
+      <c r="F185" t="n">
         <v>21.918231539801</v>
       </c>
     </row>
@@ -4578,7 +4554,7 @@
       <c r="E186" t="n">
         <v>2.843559568464182</v>
       </c>
-      <c r="F186" s="2" t="n">
+      <c r="F186" t="n">
         <v>-6.428179020953639</v>
       </c>
     </row>
@@ -4598,7 +4574,7 @@
       <c r="E187" t="n">
         <v>2.74561188762616</v>
       </c>
-      <c r="F187" s="3" t="n">
+      <c r="F187" t="n">
         <v>11.73773188710018</v>
       </c>
     </row>
@@ -4622,7 +4598,7 @@
       <c r="E188" t="n">
         <v>24.44029977167445</v>
       </c>
-      <c r="F188" s="2" t="n">
+      <c r="F188" t="n">
         <v>6.352178063909367</v>
       </c>
     </row>
@@ -4642,7 +4618,7 @@
       <c r="E189" t="n">
         <v>22.59536258124399</v>
       </c>
-      <c r="F189" s="3" t="n">
+      <c r="F189" t="n">
         <v>13.05626284806926</v>
       </c>
     </row>
@@ -4666,7 +4642,7 @@
       <c r="E190" t="n">
         <v>13.25377899782831</v>
       </c>
-      <c r="F190" s="2" t="n">
+      <c r="F190" t="n">
         <v>6.175036914247626</v>
       </c>
     </row>
@@ -4686,7 +4662,7 @@
       <c r="E191" t="n">
         <v>10.74017582058111</v>
       </c>
-      <c r="F191" s="5" t="n">
+      <c r="F191" t="n">
         <v>7.202320872136883</v>
       </c>
     </row>
@@ -4710,7 +4686,7 @@
       <c r="E192" t="n">
         <v>44.60053047657482</v>
       </c>
-      <c r="F192" s="4" t="n">
+      <c r="F192" t="n">
         <v>-6.05150820316312</v>
       </c>
     </row>
@@ -4730,7 +4706,7 @@
       <c r="E193" t="n">
         <v>43.09554964390908</v>
       </c>
-      <c r="F193" s="5" t="n">
+      <c r="F193" t="n">
         <v>-0.357475290133267</v>
       </c>
     </row>
@@ -4754,7 +4730,7 @@
       <c r="E194" t="n">
         <v>9.384015821923583</v>
       </c>
-      <c r="F194" s="2" t="n">
+      <c r="F194" t="n">
         <v>5.799500926959516</v>
       </c>
     </row>
@@ -4774,7 +4750,7 @@
       <c r="E195" t="n">
         <v>9.196496037837035</v>
       </c>
-      <c r="F195" s="3" t="n">
+      <c r="F195" t="n">
         <v>59.91806235638546</v>
       </c>
     </row>
@@ -4798,7 +4774,7 @@
       <c r="E196" t="n">
         <v>0.1940955745329077</v>
       </c>
-      <c r="F196" s="2" t="n">
+      <c r="F196" t="n">
         <v>4.943474132044954</v>
       </c>
     </row>
@@ -4818,7 +4794,7 @@
       <c r="E197" t="n">
         <v>0.1358234736615443</v>
       </c>
-      <c r="F197" s="5" t="n">
+      <c r="F197" t="n">
         <v>11.12241367705554</v>
       </c>
     </row>
@@ -4842,7 +4818,7 @@
       <c r="E198" t="n">
         <v>0.07549672917919356</v>
       </c>
-      <c r="F198" s="2" t="n">
+      <c r="F198" t="n">
         <v>4.661375232006958</v>
       </c>
     </row>
@@ -4862,7 +4838,7 @@
       <c r="E199" t="n">
         <v>0.05552130821444386</v>
       </c>
-      <c r="F199" s="4" t="n">
+      <c r="F199" t="n">
         <v>-5.590458199326393</v>
       </c>
     </row>
@@ -4886,7 +4862,7 @@
       <c r="E200" t="n">
         <v>41.13612501464005</v>
       </c>
-      <c r="F200" s="2" t="n">
+      <c r="F200" t="n">
         <v>3.912928275474013</v>
       </c>
     </row>
@@ -4906,7 +4882,7 @@
       <c r="E201" t="n">
         <v>37.82962195443426</v>
       </c>
-      <c r="F201" s="5" t="n">
+      <c r="F201" t="n">
         <v>11.12265291254577</v>
       </c>
     </row>
@@ -4930,7 +4906,7 @@
       <c r="E202" t="n">
         <v>0.02132043743887653</v>
       </c>
-      <c r="F202" s="2" t="n">
+      <c r="F202" t="n">
         <v>3.746903575341724</v>
       </c>
     </row>
@@ -4950,7 +4926,7 @@
       <c r="E203" t="n">
         <v>0.0147302148412853</v>
       </c>
-      <c r="F203" s="3" t="n">
+      <c r="F203" t="n">
         <v>19.53492277598386</v>
       </c>
     </row>
@@ -4974,7 +4950,7 @@
       <c r="E204" t="n">
         <v>6.934070356268501</v>
       </c>
-      <c r="F204" s="2" t="n">
+      <c r="F204" t="n">
         <v>3.569198155201278</v>
       </c>
     </row>
@@ -4994,7 +4970,7 @@
       <c r="E205" t="n">
         <v>6.123805368959093</v>
       </c>
-      <c r="F205" s="3" t="n">
+      <c r="F205" t="n">
         <v>12.18934106224954</v>
       </c>
     </row>
@@ -5018,7 +4994,7 @@
       <c r="E206" t="n">
         <v>0.05706129274008045</v>
       </c>
-      <c r="F206" s="2" t="n">
+      <c r="F206" t="n">
         <v>-3.565817481817142</v>
       </c>
     </row>
@@ -5038,7 +5014,7 @@
       <c r="E207" t="n">
         <v>0.0470196238065823</v>
       </c>
-      <c r="F207" s="3" t="n">
+      <c r="F207" t="n">
         <v>16.73741858917208</v>
       </c>
     </row>
@@ -5062,7 +5038,7 @@
       <c r="E208" t="n">
         <v>2.025126272508674</v>
       </c>
-      <c r="F208" s="2" t="n">
+      <c r="F208" t="n">
         <v>-3.281492499124018</v>
       </c>
     </row>
@@ -5082,7 +5058,7 @@
       <c r="E209" t="n">
         <v>1.84593866150964</v>
       </c>
-      <c r="F209" s="3" t="n">
+      <c r="F209" t="n">
         <v>13.92677239150877</v>
       </c>
     </row>
@@ -5106,7 +5082,7 @@
       <c r="E210" t="n">
         <v>47.47375390967878</v>
       </c>
-      <c r="F210" s="2" t="n">
+      <c r="F210" t="n">
         <v>3.274693155685162</v>
       </c>
     </row>
@@ -5126,7 +5102,7 @@
       <c r="E211" t="n">
         <v>44.59774309518705</v>
       </c>
-      <c r="F211" s="5" t="n">
+      <c r="F211" t="n">
         <v>10.9280349592837</v>
       </c>
     </row>
@@ -5150,7 +5126,7 @@
       <c r="E212" t="n">
         <v>0.1307418823141236</v>
       </c>
-      <c r="F212" s="2" t="n">
+      <c r="F212" t="n">
         <v>3.037529014366405</v>
       </c>
     </row>
@@ -5170,7 +5146,7 @@
       <c r="E213" t="n">
         <v>0.08556721094932931</v>
       </c>
-      <c r="F213" s="5" t="n">
+      <c r="F213" t="n">
         <v>12.10314697786544</v>
       </c>
     </row>
@@ -5194,7 +5170,7 @@
       <c r="E214" t="n">
         <v>0.1670905235913781</v>
       </c>
-      <c r="F214" s="2" t="n">
+      <c r="F214" t="n">
         <v>2.907998597462117</v>
       </c>
     </row>
@@ -5214,7 +5190,7 @@
       <c r="E215" t="n">
         <v>0.1452534686012971</v>
       </c>
-      <c r="F215" s="3" t="n">
+      <c r="F215" t="n">
         <v>12.33570991692029</v>
       </c>
     </row>
@@ -5238,7 +5214,7 @@
       <c r="E216" t="n">
         <v>0.01451915684829115</v>
       </c>
-      <c r="F216" s="3" t="n">
+      <c r="F216" t="n">
         <v>2.898216162102677</v>
       </c>
     </row>
@@ -5258,7 +5234,7 @@
       <c r="E217" t="n">
         <v>0.01319613985960079</v>
       </c>
-      <c r="F217" s="3" t="n">
+      <c r="F217" t="n">
         <v>20.53466583978908</v>
       </c>
     </row>
@@ -5282,7 +5258,7 @@
       <c r="E218" t="n">
         <v>4.943063421107881</v>
       </c>
-      <c r="F218" s="2" t="n">
+      <c r="F218" t="n">
         <v>-2.762115606032165</v>
       </c>
     </row>
@@ -5302,7 +5278,7 @@
       <c r="E219" t="n">
         <v>4.306895687834324</v>
       </c>
-      <c r="F219" s="3" t="n">
+      <c r="F219" t="n">
         <v>21.7251517512964</v>
       </c>
     </row>
@@ -5326,7 +5302,7 @@
       <c r="E220" t="n">
         <v>21.73251121401339</v>
       </c>
-      <c r="F220" s="2" t="n">
+      <c r="F220" t="n">
         <v>2.42102813409206</v>
       </c>
     </row>
@@ -5346,7 +5322,7 @@
       <c r="E221" t="n">
         <v>19.24956079633929</v>
       </c>
-      <c r="F221" s="3" t="n">
+      <c r="F221" t="n">
         <v>30.3972978434524</v>
       </c>
     </row>
@@ -5370,7 +5346,7 @@
       <c r="E222" t="n">
         <v>20.57561914194189</v>
       </c>
-      <c r="F222" s="2" t="n">
+      <c r="F222" t="n">
         <v>2.358516630917816</v>
       </c>
     </row>
@@ -5390,7 +5366,7 @@
       <c r="E223" t="n">
         <v>17.90964663085183</v>
       </c>
-      <c r="F223" s="3" t="n">
+      <c r="F223" t="n">
         <v>27.94840295307784</v>
       </c>
     </row>
@@ -5414,7 +5390,7 @@
       <c r="E224" t="n">
         <v>0.350088226012505</v>
       </c>
-      <c r="F224" s="2" t="n">
+      <c r="F224" t="n">
         <v>2.262154050767729</v>
       </c>
     </row>
@@ -5434,7 +5410,7 @@
       <c r="E225" t="n">
         <v>0.3000062628506236</v>
       </c>
-      <c r="F225" s="5" t="n">
+      <c r="F225" t="n">
         <v>10.01746270219812</v>
       </c>
     </row>
@@ -5458,7 +5434,7 @@
       <c r="E226" t="n">
         <v>32.18989238108161</v>
       </c>
-      <c r="F226" s="2" t="n">
+      <c r="F226" t="n">
         <v>2.224108396328444</v>
       </c>
     </row>
@@ -5478,7 +5454,7 @@
       <c r="E227" t="n">
         <v>27.00778226497966</v>
       </c>
-      <c r="F227" s="5" t="n">
+      <c r="F227" t="n">
         <v>6.956348827570183</v>
       </c>
     </row>
@@ -5502,7 +5478,7 @@
       <c r="E228" t="n">
         <v>4.06044831197166</v>
       </c>
-      <c r="F228" s="2" t="n">
+      <c r="F228" t="n">
         <v>2.214466843342102</v>
       </c>
     </row>
@@ -5522,7 +5498,7 @@
       <c r="E229" t="n">
         <v>3.446067720438852</v>
       </c>
-      <c r="F229" s="3" t="n">
+      <c r="F229" t="n">
         <v>23.21462477877591</v>
       </c>
     </row>
@@ -5546,7 +5522,7 @@
       <c r="E230" t="n">
         <v>0.150306032728396</v>
       </c>
-      <c r="F230" s="5" t="n">
+      <c r="F230" t="n">
         <v>-1.974921563299898</v>
       </c>
     </row>
@@ -5566,7 +5542,7 @@
       <c r="E231" t="n">
         <v>0.09356861447491503</v>
       </c>
-      <c r="F231" s="5" t="n">
+      <c r="F231" t="n">
         <v>4.000580991509802</v>
       </c>
     </row>
@@ -5590,7 +5566,7 @@
       <c r="E232" t="n">
         <v>12.33386765311571</v>
       </c>
-      <c r="F232" s="2" t="n">
+      <c r="F232" t="n">
         <v>1.902652486285068</v>
       </c>
     </row>
@@ -5610,7 +5586,7 @@
       <c r="E233" t="n">
         <v>9.251346317502227</v>
       </c>
-      <c r="F233" s="4" t="n">
+      <c r="F233" t="n">
         <v>-16.50318097104864</v>
       </c>
     </row>
@@ -5634,7 +5610,7 @@
       <c r="E234" t="n">
         <v>0.5182258886081456</v>
       </c>
-      <c r="F234" s="2" t="n">
+      <c r="F234" t="n">
         <v>-1.790016811567965</v>
       </c>
     </row>
@@ -5654,7 +5630,7 @@
       <c r="E235" t="n">
         <v>0.4652308777165046</v>
       </c>
-      <c r="F235" s="5" t="n">
+      <c r="F235" t="n">
         <v>10.3056624013451</v>
       </c>
     </row>
@@ -5678,7 +5654,7 @@
       <c r="E236" t="n">
         <v>8.821887095045611</v>
       </c>
-      <c r="F236" s="2" t="n">
+      <c r="F236" t="n">
         <v>-1.592454118619873</v>
       </c>
     </row>
@@ -5698,7 +5674,7 @@
       <c r="E237" t="n">
         <v>7.181112871979821</v>
       </c>
-      <c r="F237" s="5" t="n">
+      <c r="F237" t="n">
         <v>-5.80361489418733</v>
       </c>
     </row>
@@ -5722,7 +5698,7 @@
       <c r="E238" t="n">
         <v>9.002044964850409</v>
       </c>
-      <c r="F238" s="2" t="n">
+      <c r="F238" t="n">
         <v>-1.52823513750449</v>
       </c>
     </row>
@@ -5742,7 +5718,7 @@
       <c r="E239" t="n">
         <v>7.332561510145172</v>
       </c>
-      <c r="F239" s="5" t="n">
+      <c r="F239" t="n">
         <v>-6.827624972902278</v>
       </c>
     </row>
@@ -5766,7 +5742,7 @@
       <c r="E240" t="n">
         <v>19.35627908702781</v>
       </c>
-      <c r="F240" s="2" t="n">
+      <c r="F240" t="n">
         <v>-1.374901302200505</v>
       </c>
     </row>
@@ -5786,7 +5762,7 @@
       <c r="E241" t="n">
         <v>17.66774088746812</v>
       </c>
-      <c r="F241" s="3" t="n">
+      <c r="F241" t="n">
         <v>11.18638723995064</v>
       </c>
     </row>
@@ -5810,7 +5786,7 @@
       <c r="E242" t="n">
         <v>20.51642903537849</v>
       </c>
-      <c r="F242" s="2" t="n">
+      <c r="F242" t="n">
         <v>-1.359237966111409</v>
       </c>
     </row>
@@ -5830,7 +5806,7 @@
       <c r="E243" t="n">
         <v>18.70820507335648</v>
       </c>
-      <c r="F243" s="3" t="n">
+      <c r="F243" t="n">
         <v>27.5628940659777</v>
       </c>
     </row>
@@ -5854,7 +5830,7 @@
       <c r="E244" t="n">
         <v>13.49814251350317</v>
       </c>
-      <c r="F244" s="2" t="n">
+      <c r="F244" t="n">
         <v>-1.347229231190644</v>
       </c>
     </row>
@@ -5874,7 +5850,7 @@
       <c r="E245" t="n">
         <v>12.22872418729508</v>
       </c>
-      <c r="F245" s="3" t="n">
+      <c r="F245" t="n">
         <v>13.24904047191782</v>
       </c>
     </row>
@@ -5898,7 +5874,7 @@
       <c r="E246" t="n">
         <v>5.899123198753109</v>
       </c>
-      <c r="F246" s="2" t="n">
+      <c r="F246" t="n">
         <v>-1.312079963242104</v>
       </c>
     </row>
@@ -5918,7 +5894,7 @@
       <c r="E247" t="n">
         <v>5.168989684609575</v>
       </c>
-      <c r="F247" s="3" t="n">
+      <c r="F247" t="n">
         <v>12.71117114705869</v>
       </c>
     </row>
@@ -5942,7 +5918,7 @@
       <c r="E248" t="n">
         <v>0.2287488888078291</v>
       </c>
-      <c r="F248" s="2" t="n">
+      <c r="F248" t="n">
         <v>1.196887910154979</v>
       </c>
     </row>
@@ -5962,7 +5938,7 @@
       <c r="E249" t="n">
         <v>0.207925360006829</v>
       </c>
-      <c r="F249" s="3" t="n">
+      <c r="F249" t="n">
         <v>12.1410636137359</v>
       </c>
     </row>
@@ -5986,7 +5962,7 @@
       <c r="E250" t="n">
         <v>0.0238055036947708</v>
       </c>
-      <c r="F250" s="2" t="n">
+      <c r="F250" t="n">
         <v>-1.195998994152299</v>
       </c>
     </row>
@@ -6006,7 +5982,7 @@
       <c r="E251" t="n">
         <v>0.01793977657656616</v>
       </c>
-      <c r="F251" s="3" t="n">
+      <c r="F251" t="n">
         <v>20.80711106630305</v>
       </c>
     </row>
@@ -6030,7 +6006,7 @@
       <c r="E252" t="n">
         <v>0.2248306237521426</v>
       </c>
-      <c r="F252" s="5" t="n">
+      <c r="F252" t="n">
         <v>-1.181777450510868</v>
       </c>
     </row>
@@ -6050,7 +6026,7 @@
       <c r="E253" t="n">
         <v>0.1901088267517848</v>
       </c>
-      <c r="F253" s="2" t="n">
+      <c r="F253" t="n">
         <v>14.29217094953253</v>
       </c>
     </row>
@@ -6074,7 +6050,7 @@
       <c r="E254" t="n">
         <v>37.75007076503225</v>
       </c>
-      <c r="F254" s="2" t="n">
+      <c r="F254" t="n">
         <v>-0.8198489796756762</v>
       </c>
     </row>
@@ -6094,7 +6070,7 @@
       <c r="E255" t="n">
         <v>35.56513199931435</v>
       </c>
-      <c r="F255" s="3" t="n">
+      <c r="F255" t="n">
         <v>6.631574449468711</v>
       </c>
     </row>
@@ -6118,7 +6094,7 @@
       <c r="E256" t="n">
         <v>13.98847510130309</v>
       </c>
-      <c r="F256" s="2" t="n">
+      <c r="F256" t="n">
         <v>-0.4977240241847999</v>
       </c>
     </row>
@@ -6138,7 +6114,7 @@
       <c r="E257" t="n">
         <v>12.67908226492365</v>
       </c>
-      <c r="F257" s="3" t="n">
+      <c r="F257" t="n">
         <v>14.18170955083881</v>
       </c>
     </row>
@@ -6162,7 +6138,7 @@
       <c r="E258" t="n">
         <v>0.1213025919245322</v>
       </c>
-      <c r="F258" s="2" t="n">
+      <c r="F258" t="n">
         <v>0.2649902565700729</v>
       </c>
     </row>
@@ -6182,7 +6158,7 @@
       <c r="E259" t="n">
         <v>0.1042379215175842</v>
       </c>
-      <c r="F259" s="3" t="n">
+      <c r="F259" t="n">
         <v>19.4451310798256</v>
       </c>
     </row>
@@ -6206,7 +6182,7 @@
       <c r="E260" t="n">
         <v>5.887842165368203</v>
       </c>
-      <c r="F260" s="2" t="n">
+      <c r="F260" t="n">
         <v>0.01315643100789752</v>
       </c>
     </row>
@@ -6226,7 +6202,7 @@
       <c r="E261" t="n">
         <v>5.101179536880823</v>
       </c>
-      <c r="F261" s="5" t="n">
+      <c r="F261" t="n">
         <v>6.742439955446747</v>
       </c>
     </row>

</xml_diff>